<commit_message>
Weekly economic data update
</commit_message>
<xml_diff>
--- a/Economic_Metrics_All_Metros.xlsx
+++ b/Economic_Metrics_All_Metros.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Metric Scores" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Raw Values" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="By Rank" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Top vs Bottom" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Metric Scores" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Raw Values" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="By Rank" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Top vs Bottom" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -673,7 +673,7 @@
         </is>
       </c>
       <c r="F2" s="2" t="n">
-        <v>72.90000000000001</v>
+        <v>72.7</v>
       </c>
       <c r="G2" s="3" t="inlineStr">
         <is>
@@ -704,7 +704,7 @@
         </is>
       </c>
       <c r="F3" s="5" t="n">
-        <v>68.09999999999999</v>
+        <v>68.3</v>
       </c>
       <c r="G3" s="6" t="inlineStr">
         <is>
@@ -735,7 +735,7 @@
         </is>
       </c>
       <c r="F4" s="5" t="n">
-        <v>67</v>
+        <v>66.8</v>
       </c>
       <c r="G4" s="6" t="inlineStr">
         <is>
@@ -745,20 +745,20 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="n">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B5" s="6" t="inlineStr">
         <is>
-          <t>Hartford-West Hartford-East Hartford</t>
+          <t>Salt Lake City-Murray</t>
         </is>
       </c>
       <c r="C5" s="6" t="inlineStr">
         <is>
-          <t>Hartford</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
       <c r="D5" s="7" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E5" s="6" t="inlineStr">
         <is>
@@ -766,7 +766,7 @@
         </is>
       </c>
       <c r="F5" s="5" t="n">
-        <v>64.90000000000001</v>
+        <v>65.5</v>
       </c>
       <c r="G5" s="6" t="inlineStr">
         <is>
@@ -776,20 +776,20 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B6" s="6" t="inlineStr">
         <is>
-          <t>Milwaukee-Waukesha</t>
+          <t>Hartford-West Hartford-East Hartford</t>
         </is>
       </c>
       <c r="C6" s="6" t="inlineStr">
         <is>
-          <t>Milwaukee</t>
+          <t>Hartford</t>
         </is>
       </c>
       <c r="D6" s="7" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E6" s="6" t="inlineStr">
         <is>
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="F6" s="5" t="n">
-        <v>63.5</v>
+        <v>64.90000000000001</v>
       </c>
       <c r="G6" s="6" t="inlineStr">
         <is>
@@ -807,16 +807,16 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="n">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B7" s="6" t="inlineStr">
         <is>
-          <t>Salt Lake City-Murray</t>
+          <t>Milwaukee-Waukesha</t>
         </is>
       </c>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Milwaukee</t>
         </is>
       </c>
       <c r="D7" s="7" t="n">
@@ -828,7 +828,7 @@
         </is>
       </c>
       <c r="F7" s="5" t="n">
-        <v>64.3</v>
+        <v>63.5</v>
       </c>
       <c r="G7" s="6" t="inlineStr">
         <is>
@@ -838,16 +838,16 @@
     </row>
     <row r="8">
       <c r="A8" s="5" t="n">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B8" s="6" t="inlineStr">
         <is>
-          <t>Grand Rapids-Wyoming-Kentwood</t>
+          <t>Louisville-Jefferson County</t>
         </is>
       </c>
       <c r="C8" s="6" t="inlineStr">
         <is>
-          <t>Grand Rapids</t>
+          <t>Louisville</t>
         </is>
       </c>
       <c r="D8" s="7" t="n">
@@ -859,7 +859,7 @@
         </is>
       </c>
       <c r="F8" s="5" t="n">
-        <v>62.5</v>
+        <v>61.6</v>
       </c>
       <c r="G8" s="6" t="inlineStr">
         <is>
@@ -869,20 +869,20 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="n">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B9" s="6" t="inlineStr">
         <is>
-          <t>Louisville-Jefferson County</t>
+          <t>Grand Rapids-Wyoming-Kentwood</t>
         </is>
       </c>
       <c r="C9" s="6" t="inlineStr">
         <is>
-          <t>Louisville</t>
+          <t>Grand Rapids</t>
         </is>
       </c>
       <c r="D9" s="7" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E9" s="6" t="inlineStr">
         <is>
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="F9" s="5" t="n">
-        <v>61.4</v>
+        <v>62.5</v>
       </c>
       <c r="G9" s="6" t="inlineStr">
         <is>
@@ -921,7 +921,7 @@
         </is>
       </c>
       <c r="F10" s="8" t="n">
-        <v>59.1</v>
+        <v>59.3</v>
       </c>
       <c r="G10" s="9" t="inlineStr">
         <is>
@@ -983,7 +983,7 @@
         </is>
       </c>
       <c r="F12" s="8" t="n">
-        <v>56</v>
+        <v>56.2</v>
       </c>
       <c r="G12" s="9" t="inlineStr">
         <is>
@@ -1014,7 +1014,7 @@
         </is>
       </c>
       <c r="F13" s="8" t="n">
-        <v>55.7</v>
+        <v>55.5</v>
       </c>
       <c r="G13" s="9" t="inlineStr">
         <is>
@@ -1045,7 +1045,7 @@
         </is>
       </c>
       <c r="F14" s="8" t="n">
-        <v>56.2</v>
+        <v>56</v>
       </c>
       <c r="G14" s="9" t="inlineStr">
         <is>
@@ -1076,7 +1076,7 @@
         </is>
       </c>
       <c r="F15" s="8" t="n">
-        <v>55</v>
+        <v>55.4</v>
       </c>
       <c r="G15" s="9" t="inlineStr">
         <is>
@@ -1138,7 +1138,7 @@
         </is>
       </c>
       <c r="F17" s="8" t="n">
-        <v>54.1</v>
+        <v>54.3</v>
       </c>
       <c r="G17" s="9" t="inlineStr">
         <is>
@@ -1169,7 +1169,7 @@
         </is>
       </c>
       <c r="F18" s="8" t="n">
-        <v>53.8</v>
+        <v>53.6</v>
       </c>
       <c r="G18" s="9" t="inlineStr">
         <is>
@@ -1200,7 +1200,7 @@
         </is>
       </c>
       <c r="F19" s="8" t="n">
-        <v>53.7</v>
+        <v>53.5</v>
       </c>
       <c r="G19" s="9" t="inlineStr">
         <is>
@@ -1231,7 +1231,7 @@
         </is>
       </c>
       <c r="F20" s="8" t="n">
-        <v>52.8</v>
+        <v>53.2</v>
       </c>
       <c r="G20" s="9" t="inlineStr">
         <is>
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="F21" s="8" t="n">
-        <v>52.9</v>
+        <v>52.7</v>
       </c>
       <c r="G21" s="9" t="inlineStr">
         <is>
@@ -1293,7 +1293,7 @@
         </is>
       </c>
       <c r="F22" s="8" t="n">
-        <v>52.2</v>
+        <v>51.8</v>
       </c>
       <c r="G22" s="9" t="inlineStr">
         <is>
@@ -1355,7 +1355,7 @@
         </is>
       </c>
       <c r="F24" s="8" t="n">
-        <v>52.4</v>
+        <v>52</v>
       </c>
       <c r="G24" s="9" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
         </is>
       </c>
       <c r="D25" s="10" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E25" s="9" t="inlineStr">
         <is>
@@ -1386,7 +1386,7 @@
         </is>
       </c>
       <c r="F25" s="8" t="n">
-        <v>50.4</v>
+        <v>50.6</v>
       </c>
       <c r="G25" s="9" t="inlineStr">
         <is>
@@ -1396,16 +1396,16 @@
     </row>
     <row r="26">
       <c r="A26" s="11" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B26" s="12" t="inlineStr">
         <is>
-          <t>Detroit-Warren-Dearborn</t>
+          <t>Boston-Cambridge-Newton</t>
         </is>
       </c>
       <c r="C26" s="12" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Boston</t>
         </is>
       </c>
       <c r="D26" s="13" t="n">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="F26" s="11" t="n">
-        <v>49.7</v>
+        <v>49.8</v>
       </c>
       <c r="G26" s="12" t="inlineStr">
         <is>
@@ -1426,64 +1426,64 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="8" t="n">
+      <c r="A27" s="11" t="n">
+        <v>14</v>
+      </c>
+      <c r="B27" s="12" t="inlineStr">
+        <is>
+          <t>Detroit-Warren-Dearborn</t>
+        </is>
+      </c>
+      <c r="C27" s="12" t="inlineStr">
+        <is>
+          <t>Detroit</t>
+        </is>
+      </c>
+      <c r="D27" s="13" t="n">
+        <v>50</v>
+      </c>
+      <c r="E27" s="12" t="inlineStr">
+        <is>
+          <t>B-</t>
+        </is>
+      </c>
+      <c r="F27" s="11" t="n">
+        <v>49.9</v>
+      </c>
+      <c r="G27" s="12" t="inlineStr">
+        <is>
+          <t>Below Average</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="B27" s="9" t="inlineStr">
+      <c r="B28" s="9" t="inlineStr">
         <is>
           <t>Austin-Round Rock-San Marcos</t>
         </is>
       </c>
-      <c r="C27" s="9" t="inlineStr">
+      <c r="C28" s="9" t="inlineStr">
         <is>
           <t>Austin</t>
         </is>
       </c>
-      <c r="D27" s="10" t="n">
+      <c r="D28" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="E27" s="9" t="inlineStr">
+      <c r="E28" s="9" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="F27" s="8" t="n">
+      <c r="F28" s="8" t="n">
         <v>50.3</v>
       </c>
-      <c r="G27" s="9" t="inlineStr">
+      <c r="G28" s="9" t="inlineStr">
         <is>
           <t>Average</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="11" t="n">
-        <v>11</v>
-      </c>
-      <c r="B28" s="12" t="inlineStr">
-        <is>
-          <t>Boston-Cambridge-Newton</t>
-        </is>
-      </c>
-      <c r="C28" s="12" t="inlineStr">
-        <is>
-          <t>Boston</t>
-        </is>
-      </c>
-      <c r="D28" s="13" t="n">
-        <v>49</v>
-      </c>
-      <c r="E28" s="12" t="inlineStr">
-        <is>
-          <t>B-</t>
-        </is>
-      </c>
-      <c r="F28" s="11" t="n">
-        <v>49.4</v>
-      </c>
-      <c r="G28" s="12" t="inlineStr">
-        <is>
-          <t>Below Average</t>
         </is>
       </c>
     </row>
@@ -1510,7 +1510,7 @@
         </is>
       </c>
       <c r="F29" s="11" t="n">
-        <v>48.6</v>
+        <v>49.4</v>
       </c>
       <c r="G29" s="12" t="inlineStr">
         <is>
@@ -1541,7 +1541,7 @@
         </is>
       </c>
       <c r="F30" s="11" t="n">
-        <v>49.2</v>
+        <v>49</v>
       </c>
       <c r="G30" s="12" t="inlineStr">
         <is>
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="F31" s="11" t="n">
-        <v>48.1</v>
+        <v>48.5</v>
       </c>
       <c r="G31" s="12" t="inlineStr">
         <is>
@@ -1582,16 +1582,16 @@
     </row>
     <row r="32">
       <c r="A32" s="11" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B32" s="12" t="inlineStr">
         <is>
-          <t>Phoenix-Mesa-Chandler</t>
+          <t>Tampa-St. Petersburg-Clearwater</t>
         </is>
       </c>
       <c r="C32" s="12" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="D32" s="13" t="n">
@@ -1603,7 +1603,7 @@
         </is>
       </c>
       <c r="F32" s="11" t="n">
-        <v>46.6</v>
+        <v>47.2</v>
       </c>
       <c r="G32" s="12" t="inlineStr">
         <is>
@@ -1613,20 +1613,20 @@
     </row>
     <row r="33">
       <c r="A33" s="11" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B33" s="12" t="inlineStr">
         <is>
-          <t>Tampa-St. Petersburg-Clearwater</t>
+          <t>Washington-Arlington-Alexandria</t>
         </is>
       </c>
       <c r="C33" s="12" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Washington DC</t>
         </is>
       </c>
       <c r="D33" s="13" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E33" s="12" t="inlineStr">
         <is>
@@ -1634,7 +1634,7 @@
         </is>
       </c>
       <c r="F33" s="11" t="n">
-        <v>47.2</v>
+        <v>46.1</v>
       </c>
       <c r="G33" s="12" t="inlineStr">
         <is>
@@ -1644,16 +1644,16 @@
     </row>
     <row r="34">
       <c r="A34" s="11" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B34" s="12" t="inlineStr">
         <is>
-          <t>Washington-Arlington-Alexandria</t>
+          <t>Phoenix-Mesa-Chandler</t>
         </is>
       </c>
       <c r="C34" s="12" t="inlineStr">
         <is>
-          <t>Washington DC</t>
+          <t>Phoenix</t>
         </is>
       </c>
       <c r="D34" s="13" t="n">
@@ -1665,7 +1665,7 @@
         </is>
       </c>
       <c r="F34" s="11" t="n">
-        <v>46.1</v>
+        <v>46.4</v>
       </c>
       <c r="G34" s="12" t="inlineStr">
         <is>
@@ -1688,7 +1688,7 @@
         </is>
       </c>
       <c r="D35" s="13" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E35" s="12" t="inlineStr">
         <is>
@@ -1696,7 +1696,7 @@
         </is>
       </c>
       <c r="F35" s="11" t="n">
-        <v>44.6</v>
+        <v>44.4</v>
       </c>
       <c r="G35" s="12" t="inlineStr">
         <is>
@@ -1719,7 +1719,7 @@
         </is>
       </c>
       <c r="D36" s="13" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E36" s="12" t="inlineStr">
         <is>
@@ -1727,7 +1727,7 @@
         </is>
       </c>
       <c r="F36" s="11" t="n">
-        <v>44.7</v>
+        <v>43.9</v>
       </c>
       <c r="G36" s="12" t="inlineStr">
         <is>
@@ -1758,7 +1758,7 @@
         </is>
       </c>
       <c r="F37" s="11" t="n">
-        <v>42.1</v>
+        <v>42.5</v>
       </c>
       <c r="G37" s="12" t="inlineStr">
         <is>
@@ -1789,7 +1789,7 @@
         </is>
       </c>
       <c r="F38" s="11" t="n">
-        <v>42.5</v>
+        <v>41.7</v>
       </c>
       <c r="G38" s="12" t="inlineStr">
         <is>
@@ -1799,16 +1799,16 @@
     </row>
     <row r="39">
       <c r="A39" s="11" t="n">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B39" s="12" t="inlineStr">
         <is>
-          <t>Orlando-Kissimmee-Sanford</t>
+          <t>San Jose-Sunnyvale-Santa Clara</t>
         </is>
       </c>
       <c r="C39" s="12" t="inlineStr">
         <is>
-          <t>Orlando</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="D39" s="13" t="n">
@@ -1820,7 +1820,7 @@
         </is>
       </c>
       <c r="F39" s="11" t="n">
-        <v>41.4</v>
+        <v>40.7</v>
       </c>
       <c r="G39" s="12" t="inlineStr">
         <is>
@@ -1830,78 +1830,78 @@
     </row>
     <row r="40">
       <c r="A40" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="B40" s="12" t="inlineStr">
+        <is>
+          <t>Orlando-Kissimmee-Sanford</t>
+        </is>
+      </c>
+      <c r="C40" s="12" t="inlineStr">
+        <is>
+          <t>Orlando</t>
+        </is>
+      </c>
+      <c r="D40" s="13" t="n">
+        <v>40</v>
+      </c>
+      <c r="E40" s="12" t="inlineStr">
+        <is>
+          <t>B-</t>
+        </is>
+      </c>
+      <c r="F40" s="11" t="n">
+        <v>40.4</v>
+      </c>
+      <c r="G40" s="12" t="inlineStr">
+        <is>
+          <t>Below Average</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="11" t="n">
         <v>38</v>
       </c>
-      <c r="B40" s="12" t="inlineStr">
+      <c r="B41" s="12" t="inlineStr">
         <is>
           <t>Jacksonville</t>
         </is>
       </c>
-      <c r="C40" s="12" t="inlineStr">
+      <c r="C41" s="12" t="inlineStr">
         <is>
           <t>Jacksonville</t>
         </is>
       </c>
-      <c r="D40" s="13" t="n">
-        <v>41</v>
-      </c>
-      <c r="E40" s="12" t="inlineStr">
+      <c r="D41" s="13" t="n">
+        <v>40</v>
+      </c>
+      <c r="E41" s="12" t="inlineStr">
         <is>
           <t>B-</t>
         </is>
       </c>
-      <c r="F40" s="11" t="n">
-        <v>41.4</v>
-      </c>
-      <c r="G40" s="12" t="inlineStr">
+      <c r="F41" s="11" t="n">
+        <v>40</v>
+      </c>
+      <c r="G41" s="12" t="inlineStr">
         <is>
           <t>Below Average</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="14" t="n">
-        <v>21</v>
-      </c>
-      <c r="B41" s="15" t="inlineStr">
-        <is>
-          <t>Charlotte-Concord-Gastonia</t>
-        </is>
-      </c>
-      <c r="C41" s="15" t="inlineStr">
-        <is>
-          <t>Charlotte</t>
-        </is>
-      </c>
-      <c r="D41" s="16" t="n">
-        <v>39</v>
-      </c>
-      <c r="E41" s="15" t="inlineStr">
-        <is>
-          <t>C+</t>
-        </is>
-      </c>
-      <c r="F41" s="14" t="n">
-        <v>39.1</v>
-      </c>
-      <c r="G41" s="15" t="inlineStr">
-        <is>
-          <t>Poor</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="14" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B42" s="15" t="inlineStr">
         <is>
-          <t>San Jose-Sunnyvale-Santa Clara</t>
+          <t>Charlotte-Concord-Gastonia</t>
         </is>
       </c>
       <c r="C42" s="15" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="D42" s="16" t="n">
@@ -1913,7 +1913,7 @@
         </is>
       </c>
       <c r="F42" s="14" t="n">
-        <v>39.3</v>
+        <v>38.9</v>
       </c>
       <c r="G42" s="15" t="inlineStr">
         <is>
@@ -1923,16 +1923,16 @@
     </row>
     <row r="43">
       <c r="A43" s="14" t="n">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="B43" s="15" t="inlineStr">
         <is>
-          <t>Las Vegas-Henderson-North Las Vegas</t>
+          <t>Fresno</t>
         </is>
       </c>
       <c r="C43" s="15" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Fresno</t>
         </is>
       </c>
       <c r="D43" s="16" t="n">
@@ -1944,7 +1944,7 @@
         </is>
       </c>
       <c r="F43" s="14" t="n">
-        <v>34.6</v>
+        <v>35.2</v>
       </c>
       <c r="G43" s="15" t="inlineStr">
         <is>
@@ -1954,20 +1954,20 @@
     </row>
     <row r="44">
       <c r="A44" s="14" t="n">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="B44" s="15" t="inlineStr">
         <is>
-          <t>Fresno</t>
+          <t>Las Vegas-Henderson-North Las Vegas</t>
         </is>
       </c>
       <c r="C44" s="15" t="inlineStr">
         <is>
-          <t>Fresno</t>
+          <t>Las Vegas</t>
         </is>
       </c>
       <c r="D44" s="16" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E44" s="15" t="inlineStr">
         <is>
@@ -1975,7 +1975,7 @@
         </is>
       </c>
       <c r="F44" s="14" t="n">
-        <v>34.6</v>
+        <v>33.8</v>
       </c>
       <c r="G44" s="15" t="inlineStr">
         <is>
@@ -2037,7 +2037,7 @@
         </is>
       </c>
       <c r="F46" s="14" t="n">
-        <v>30.5</v>
+        <v>30.3</v>
       </c>
       <c r="G46" s="15" t="inlineStr">
         <is>
@@ -2047,16 +2047,16 @@
     </row>
     <row r="47">
       <c r="A47" s="17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B47" s="18" t="inlineStr">
         <is>
-          <t>New York Newark-Jersey City</t>
+          <t>Los Angeles-Long Beach-Anaheim</t>
         </is>
       </c>
       <c r="C47" s="18" t="inlineStr">
         <is>
-          <t>New York</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="D47" s="19" t="n">
@@ -2068,7 +2068,7 @@
         </is>
       </c>
       <c r="F47" s="17" t="n">
-        <v>27.5</v>
+        <v>28.1</v>
       </c>
       <c r="G47" s="18" t="inlineStr">
         <is>
@@ -2078,20 +2078,20 @@
     </row>
     <row r="48">
       <c r="A48" s="17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B48" s="18" t="inlineStr">
         <is>
-          <t>Los Angeles-Long Beach-Anaheim</t>
+          <t>New York Newark-Jersey City</t>
         </is>
       </c>
       <c r="C48" s="18" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>New York</t>
         </is>
       </c>
       <c r="D48" s="19" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E48" s="18" t="inlineStr">
         <is>
@@ -2099,7 +2099,7 @@
         </is>
       </c>
       <c r="F48" s="17" t="n">
-        <v>27.5</v>
+        <v>27.3</v>
       </c>
       <c r="G48" s="18" t="inlineStr">
         <is>
@@ -2130,7 +2130,7 @@
         </is>
       </c>
       <c r="F49" s="17" t="n">
-        <v>24</v>
+        <v>24.2</v>
       </c>
       <c r="G49" s="18" t="inlineStr">
         <is>
@@ -2161,7 +2161,7 @@
         </is>
       </c>
       <c r="F50" s="17" t="n">
-        <v>24.2</v>
+        <v>24</v>
       </c>
       <c r="G50" s="18" t="inlineStr">
         <is>
@@ -2192,7 +2192,7 @@
         </is>
       </c>
       <c r="F51" s="20" t="n">
-        <v>19.5</v>
+        <v>19.9</v>
       </c>
       <c r="G51" s="21" t="inlineStr">
         <is>
@@ -2336,7 +2336,7 @@
         <v>70</v>
       </c>
       <c r="J2" s="25" t="n">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K2" s="25" t="n">
         <v>68</v>
@@ -2376,7 +2376,7 @@
         <v>58</v>
       </c>
       <c r="J3" s="24" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K3" s="25" t="n">
         <v>64</v>
@@ -2416,7 +2416,7 @@
         <v>84</v>
       </c>
       <c r="J4" s="25" t="n">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K4" s="25" t="n">
         <v>58</v>
@@ -2428,201 +2428,201 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Hartford-West Hartford-East Hartford</t>
+          <t>Salt Lake City-Murray</t>
         </is>
       </c>
       <c r="B5" s="23" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C5" s="24" t="n">
+        <v>74</v>
+      </c>
+      <c r="D5" s="24" t="n">
+        <v>94</v>
+      </c>
+      <c r="E5" s="26" t="n">
+        <v>40</v>
+      </c>
+      <c r="F5" s="26" t="n">
+        <v>30</v>
+      </c>
+      <c r="G5" s="24" t="n">
         <v>96</v>
       </c>
-      <c r="D5" s="25" t="n">
-        <v>52</v>
-      </c>
-      <c r="E5" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="F5" s="24" t="n">
-        <v>84</v>
-      </c>
-      <c r="G5" s="25" t="n">
-        <v>54</v>
-      </c>
-      <c r="H5" s="26" t="n">
-        <v>34</v>
+      <c r="H5" s="24" t="n">
+        <v>90</v>
       </c>
       <c r="I5" s="24" t="n">
-        <v>80</v>
-      </c>
-      <c r="J5" s="24" t="n">
-        <v>98</v>
-      </c>
-      <c r="K5" s="25" t="n">
-        <v>54</v>
-      </c>
-      <c r="L5" s="24" t="n">
-        <v>96</v>
+        <v>86</v>
+      </c>
+      <c r="J5" s="25" t="n">
+        <v>50</v>
+      </c>
+      <c r="K5" s="26" t="n">
+        <v>44</v>
+      </c>
+      <c r="L5" s="26" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Milwaukee-Waukesha</t>
+          <t>Hartford-West Hartford-East Hartford</t>
         </is>
       </c>
       <c r="B6" s="23" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C6" s="24" t="n">
-        <v>76</v>
-      </c>
-      <c r="D6" s="26" t="n">
-        <v>42</v>
+        <v>96</v>
+      </c>
+      <c r="D6" s="25" t="n">
+        <v>52</v>
       </c>
       <c r="E6" s="26" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="F6" s="24" t="n">
-        <v>92</v>
-      </c>
-      <c r="G6" s="26" t="n">
-        <v>18</v>
-      </c>
-      <c r="H6" s="25" t="n">
-        <v>60</v>
-      </c>
-      <c r="I6" s="26" t="n">
-        <v>32</v>
+        <v>84</v>
+      </c>
+      <c r="G6" s="25" t="n">
+        <v>54</v>
+      </c>
+      <c r="H6" s="26" t="n">
+        <v>34</v>
+      </c>
+      <c r="I6" s="24" t="n">
+        <v>80</v>
       </c>
       <c r="J6" s="24" t="n">
-        <v>94</v>
-      </c>
-      <c r="K6" s="24" t="n">
+        <v>98</v>
+      </c>
+      <c r="K6" s="25" t="n">
+        <v>54</v>
+      </c>
+      <c r="L6" s="24" t="n">
         <v>96</v>
-      </c>
-      <c r="L6" s="24" t="n">
-        <v>98</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Salt Lake City-Murray</t>
+          <t>Milwaukee-Waukesha</t>
         </is>
       </c>
       <c r="B7" s="23" t="n">
         <v>64</v>
       </c>
       <c r="C7" s="24" t="n">
-        <v>74</v>
-      </c>
-      <c r="D7" s="24" t="n">
+        <v>76</v>
+      </c>
+      <c r="D7" s="26" t="n">
+        <v>42</v>
+      </c>
+      <c r="E7" s="26" t="n">
+        <v>26</v>
+      </c>
+      <c r="F7" s="24" t="n">
+        <v>92</v>
+      </c>
+      <c r="G7" s="26" t="n">
+        <v>18</v>
+      </c>
+      <c r="H7" s="25" t="n">
+        <v>60</v>
+      </c>
+      <c r="I7" s="26" t="n">
+        <v>32</v>
+      </c>
+      <c r="J7" s="24" t="n">
         <v>94</v>
       </c>
-      <c r="E7" s="26" t="n">
-        <v>40</v>
-      </c>
-      <c r="F7" s="26" t="n">
-        <v>30</v>
-      </c>
-      <c r="G7" s="24" t="n">
+      <c r="K7" s="24" t="n">
         <v>96</v>
       </c>
-      <c r="H7" s="24" t="n">
-        <v>90</v>
-      </c>
-      <c r="I7" s="24" t="n">
-        <v>86</v>
-      </c>
-      <c r="J7" s="26" t="n">
-        <v>38</v>
-      </c>
-      <c r="K7" s="26" t="n">
-        <v>44</v>
-      </c>
-      <c r="L7" s="26" t="n">
-        <v>30</v>
+      <c r="L7" s="24" t="n">
+        <v>98</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Grand Rapids-Wyoming-Kentwood</t>
+          <t>Louisville-Jefferson County</t>
         </is>
       </c>
       <c r="B8" s="23" t="n">
         <v>62</v>
       </c>
-      <c r="C8" s="26" t="n">
-        <v>20</v>
-      </c>
-      <c r="D8" s="25" t="n">
+      <c r="C8" s="25" t="n">
         <v>66</v>
       </c>
-      <c r="E8" s="25" t="n">
-        <v>54</v>
+      <c r="D8" s="26" t="n">
+        <v>30</v>
+      </c>
+      <c r="E8" s="26" t="n">
+        <v>30</v>
       </c>
       <c r="F8" s="24" t="n">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G8" s="26" t="n">
-        <v>24</v>
-      </c>
-      <c r="H8" s="24" t="n">
+        <v>34</v>
+      </c>
+      <c r="H8" s="25" t="n">
+        <v>52</v>
+      </c>
+      <c r="I8" s="24" t="n">
+        <v>82</v>
+      </c>
+      <c r="J8" s="24" t="n">
         <v>78</v>
       </c>
-      <c r="I8" s="26" t="n">
-        <v>38</v>
-      </c>
-      <c r="J8" s="24" t="n">
-        <v>90</v>
-      </c>
       <c r="K8" s="24" t="n">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="L8" s="24" t="n">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Louisville-Jefferson County</t>
+          <t>Grand Rapids-Wyoming-Kentwood</t>
         </is>
       </c>
       <c r="B9" s="23" t="n">
-        <v>61</v>
-      </c>
-      <c r="C9" s="25" t="n">
+        <v>62</v>
+      </c>
+      <c r="C9" s="26" t="n">
+        <v>20</v>
+      </c>
+      <c r="D9" s="25" t="n">
         <v>66</v>
       </c>
-      <c r="D9" s="26" t="n">
-        <v>30</v>
-      </c>
-      <c r="E9" s="26" t="n">
-        <v>30</v>
+      <c r="E9" s="25" t="n">
+        <v>54</v>
       </c>
       <c r="F9" s="24" t="n">
+        <v>94</v>
+      </c>
+      <c r="G9" s="26" t="n">
+        <v>24</v>
+      </c>
+      <c r="H9" s="24" t="n">
+        <v>78</v>
+      </c>
+      <c r="I9" s="26" t="n">
+        <v>38</v>
+      </c>
+      <c r="J9" s="24" t="n">
         <v>90</v>
       </c>
-      <c r="G9" s="26" t="n">
-        <v>34</v>
-      </c>
-      <c r="H9" s="25" t="n">
-        <v>52</v>
-      </c>
-      <c r="I9" s="24" t="n">
-        <v>82</v>
-      </c>
-      <c r="J9" s="24" t="n">
-        <v>76</v>
-      </c>
       <c r="K9" s="24" t="n">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="L9" s="24" t="n">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10">
@@ -2656,7 +2656,7 @@
         <v>76</v>
       </c>
       <c r="J10" s="26" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K10" s="25" t="n">
         <v>66</v>
@@ -2736,7 +2736,7 @@
         <v>68</v>
       </c>
       <c r="J12" s="24" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="K12" s="24" t="n">
         <v>80</v>
@@ -2776,7 +2776,7 @@
         <v>60</v>
       </c>
       <c r="J13" s="24" t="n">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K13" s="24" t="n">
         <v>90</v>
@@ -2816,7 +2816,7 @@
         <v>16</v>
       </c>
       <c r="J14" s="25" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K14" s="26" t="n">
         <v>42</v>
@@ -2856,7 +2856,7 @@
         <v>74</v>
       </c>
       <c r="J15" s="26" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="K15" s="26" t="n">
         <v>8</v>
@@ -2936,7 +2936,7 @@
         <v>26</v>
       </c>
       <c r="J17" s="26" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K17" s="26" t="n">
         <v>36</v>
@@ -2976,7 +2976,7 @@
         <v>42</v>
       </c>
       <c r="J18" s="26" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K18" s="25" t="n">
         <v>52</v>
@@ -3016,7 +3016,7 @@
         <v>78</v>
       </c>
       <c r="J19" s="26" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K19" s="24" t="n">
         <v>98</v>
@@ -3056,7 +3056,7 @@
         <v>34</v>
       </c>
       <c r="J20" s="24" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="K20" s="24" t="n">
         <v>74</v>
@@ -3095,8 +3095,8 @@
       <c r="I21" s="25" t="n">
         <v>52</v>
       </c>
-      <c r="J21" s="24" t="n">
-        <v>70</v>
+      <c r="J21" s="25" t="n">
+        <v>68</v>
       </c>
       <c r="K21" s="24" t="n">
         <v>70</v>
@@ -3136,7 +3136,7 @@
         <v>56</v>
       </c>
       <c r="J22" s="26" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K22" s="26" t="n">
         <v>30</v>
@@ -3216,7 +3216,7 @@
         <v>50</v>
       </c>
       <c r="J24" s="24" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="K24" s="25" t="n">
         <v>50</v>
@@ -3232,7 +3232,7 @@
         </is>
       </c>
       <c r="B25" s="23" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C25" s="26" t="n">
         <v>32</v>
@@ -3256,7 +3256,7 @@
         <v>72</v>
       </c>
       <c r="J25" s="26" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K25" s="25" t="n">
         <v>62</v>
@@ -3268,121 +3268,121 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Detroit-Warren-Dearborn</t>
+          <t>Boston-Cambridge-Newton</t>
         </is>
       </c>
       <c r="B26" s="23" t="n">
         <v>50</v>
       </c>
-      <c r="C26" s="26" t="n">
-        <v>48</v>
-      </c>
-      <c r="D26" s="26" t="n">
+      <c r="C26" s="24" t="n">
+        <v>70</v>
+      </c>
+      <c r="D26" s="24" t="n">
+        <v>84</v>
+      </c>
+      <c r="E26" s="26" t="n">
         <v>22</v>
       </c>
-      <c r="E26" s="25" t="n">
-        <v>56</v>
-      </c>
-      <c r="F26" s="25" t="n">
-        <v>58</v>
-      </c>
-      <c r="G26" s="26" t="n">
+      <c r="F26" s="26" t="n">
+        <v>10</v>
+      </c>
+      <c r="G26" s="25" t="n">
+        <v>66</v>
+      </c>
+      <c r="H26" s="26" t="n">
         <v>20</v>
       </c>
-      <c r="H26" s="24" t="n">
-        <v>70</v>
-      </c>
-      <c r="I26" s="24" t="n">
-        <v>88</v>
+      <c r="I26" s="26" t="n">
+        <v>18</v>
       </c>
       <c r="J26" s="26" t="n">
-        <v>34</v>
-      </c>
-      <c r="K26" s="26" t="n">
         <v>40</v>
       </c>
+      <c r="K26" s="24" t="n">
+        <v>78</v>
+      </c>
       <c r="L26" s="24" t="n">
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Austin-Round Rock-San Marcos</t>
+          <t>Detroit-Warren-Dearborn</t>
         </is>
       </c>
       <c r="B27" s="23" t="n">
         <v>50</v>
       </c>
-      <c r="C27" s="24" t="n">
+      <c r="C27" s="26" t="n">
+        <v>48</v>
+      </c>
+      <c r="D27" s="26" t="n">
+        <v>22</v>
+      </c>
+      <c r="E27" s="25" t="n">
+        <v>56</v>
+      </c>
+      <c r="F27" s="25" t="n">
+        <v>58</v>
+      </c>
+      <c r="G27" s="26" t="n">
+        <v>20</v>
+      </c>
+      <c r="H27" s="24" t="n">
         <v>70</v>
       </c>
-      <c r="D27" s="24" t="n">
-        <v>96</v>
-      </c>
-      <c r="E27" s="25" t="n">
-        <v>62</v>
-      </c>
-      <c r="F27" s="25" t="n">
-        <v>68</v>
-      </c>
-      <c r="G27" s="25" t="n">
-        <v>56</v>
-      </c>
-      <c r="H27" s="24" t="n">
-        <v>86</v>
-      </c>
-      <c r="I27" s="26" t="n">
-        <v>6</v>
-      </c>
-      <c r="J27" s="27" t="n">
-        <v>0</v>
+      <c r="I27" s="24" t="n">
+        <v>88</v>
+      </c>
+      <c r="J27" s="26" t="n">
+        <v>36</v>
       </c>
       <c r="K27" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="L27" s="26" t="n">
-        <v>4</v>
+        <v>40</v>
+      </c>
+      <c r="L27" s="24" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Boston-Cambridge-Newton</t>
+          <t>Austin-Round Rock-San Marcos</t>
         </is>
       </c>
       <c r="B28" s="23" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C28" s="24" t="n">
         <v>70</v>
       </c>
       <c r="D28" s="24" t="n">
-        <v>84</v>
-      </c>
-      <c r="E28" s="26" t="n">
-        <v>22</v>
-      </c>
-      <c r="F28" s="26" t="n">
-        <v>10</v>
+        <v>96</v>
+      </c>
+      <c r="E28" s="25" t="n">
+        <v>62</v>
+      </c>
+      <c r="F28" s="25" t="n">
+        <v>68</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>66</v>
-      </c>
-      <c r="H28" s="26" t="n">
-        <v>20</v>
+        <v>56</v>
+      </c>
+      <c r="H28" s="24" t="n">
+        <v>86</v>
       </c>
       <c r="I28" s="26" t="n">
-        <v>18</v>
-      </c>
-      <c r="J28" s="26" t="n">
-        <v>36</v>
-      </c>
-      <c r="K28" s="24" t="n">
-        <v>78</v>
-      </c>
-      <c r="L28" s="24" t="n">
-        <v>92</v>
+        <v>6</v>
+      </c>
+      <c r="J28" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="L28" s="26" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="29">
@@ -3415,8 +3415,8 @@
       <c r="I29" s="26" t="n">
         <v>12</v>
       </c>
-      <c r="J29" s="25" t="n">
-        <v>64</v>
+      <c r="J29" s="24" t="n">
+        <v>72</v>
       </c>
       <c r="K29" s="24" t="n">
         <v>86</v>
@@ -3456,7 +3456,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="24" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K30" s="24" t="n">
         <v>92</v>
@@ -3496,7 +3496,7 @@
         <v>94</v>
       </c>
       <c r="J31" s="26" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K31" s="26" t="n">
         <v>12</v>
@@ -3508,121 +3508,121 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Phoenix-Mesa-Chandler</t>
+          <t>Tampa-St. Petersburg-Clearwater</t>
         </is>
       </c>
       <c r="B32" s="23" t="n">
         <v>47</v>
       </c>
-      <c r="C32" s="25" t="n">
-        <v>60</v>
-      </c>
-      <c r="D32" s="25" t="n">
-        <v>64</v>
-      </c>
-      <c r="E32" s="25" t="n">
-        <v>68</v>
-      </c>
-      <c r="F32" s="26" t="n">
-        <v>40</v>
-      </c>
-      <c r="G32" s="25" t="n">
-        <v>52</v>
+      <c r="C32" s="26" t="n">
+        <v>42</v>
+      </c>
+      <c r="D32" s="26" t="n">
+        <v>10</v>
+      </c>
+      <c r="E32" s="24" t="n">
+        <v>88</v>
+      </c>
+      <c r="F32" s="25" t="n">
+        <v>66</v>
+      </c>
+      <c r="G32" s="24" t="n">
+        <v>70</v>
       </c>
       <c r="H32" s="24" t="n">
-        <v>70</v>
-      </c>
-      <c r="I32" s="26" t="n">
-        <v>24</v>
+        <v>78</v>
+      </c>
+      <c r="I32" s="25" t="n">
+        <v>66</v>
       </c>
       <c r="J32" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="K32" s="25" t="n">
+        <v>56</v>
+      </c>
+      <c r="L32" s="26" t="n">
         <v>6</v>
-      </c>
-      <c r="K32" s="26" t="n">
-        <v>28</v>
-      </c>
-      <c r="L32" s="26" t="n">
-        <v>36</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Tampa-St. Petersburg-Clearwater</t>
+          <t>Washington-Arlington-Alexandria</t>
         </is>
       </c>
       <c r="B33" s="23" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" s="26" t="n">
-        <v>42</v>
-      </c>
-      <c r="D33" s="26" t="n">
-        <v>10</v>
-      </c>
-      <c r="E33" s="24" t="n">
-        <v>88</v>
-      </c>
-      <c r="F33" s="25" t="n">
-        <v>66</v>
-      </c>
-      <c r="G33" s="24" t="n">
+        <v>48</v>
+      </c>
+      <c r="D33" s="24" t="n">
+        <v>80</v>
+      </c>
+      <c r="E33" s="26" t="n">
+        <v>18</v>
+      </c>
+      <c r="F33" s="26" t="n">
+        <v>36</v>
+      </c>
+      <c r="G33" s="26" t="n">
+        <v>46</v>
+      </c>
+      <c r="H33" s="24" t="n">
         <v>70</v>
       </c>
-      <c r="H33" s="24" t="n">
-        <v>78</v>
-      </c>
       <c r="I33" s="25" t="n">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="J33" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="K33" s="25" t="n">
-        <v>56</v>
-      </c>
-      <c r="L33" s="26" t="n">
-        <v>6</v>
+        <v>26</v>
+      </c>
+      <c r="K33" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" s="24" t="n">
+        <v>84</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Washington-Arlington-Alexandria</t>
+          <t>Phoenix-Mesa-Chandler</t>
         </is>
       </c>
       <c r="B34" s="23" t="n">
         <v>46</v>
       </c>
-      <c r="C34" s="26" t="n">
-        <v>48</v>
-      </c>
-      <c r="D34" s="24" t="n">
-        <v>80</v>
-      </c>
-      <c r="E34" s="26" t="n">
-        <v>18</v>
+      <c r="C34" s="25" t="n">
+        <v>60</v>
+      </c>
+      <c r="D34" s="25" t="n">
+        <v>64</v>
+      </c>
+      <c r="E34" s="25" t="n">
+        <v>68</v>
       </c>
       <c r="F34" s="26" t="n">
-        <v>36</v>
-      </c>
-      <c r="G34" s="26" t="n">
-        <v>46</v>
+        <v>40</v>
+      </c>
+      <c r="G34" s="25" t="n">
+        <v>52</v>
       </c>
       <c r="H34" s="24" t="n">
         <v>70</v>
       </c>
-      <c r="I34" s="25" t="n">
-        <v>54</v>
+      <c r="I34" s="26" t="n">
+        <v>24</v>
       </c>
       <c r="J34" s="26" t="n">
-        <v>26</v>
-      </c>
-      <c r="K34" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="L34" s="24" t="n">
-        <v>84</v>
+        <v>4</v>
+      </c>
+      <c r="K34" s="26" t="n">
+        <v>28</v>
+      </c>
+      <c r="L34" s="26" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="35">
@@ -3632,7 +3632,7 @@
         </is>
       </c>
       <c r="B35" s="23" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="26" t="n">
         <v>16</v>
@@ -3656,7 +3656,7 @@
         <v>40</v>
       </c>
       <c r="J35" s="25" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K35" s="26" t="n">
         <v>32</v>
@@ -3672,7 +3672,7 @@
         </is>
       </c>
       <c r="B36" s="23" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C36" s="26" t="n">
         <v>32</v>
@@ -3695,8 +3695,8 @@
       <c r="I36" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="J36" s="25" t="n">
-        <v>50</v>
+      <c r="J36" s="26" t="n">
+        <v>42</v>
       </c>
       <c r="K36" s="25" t="n">
         <v>60</v>
@@ -3735,8 +3735,8 @@
       <c r="I37" s="26" t="n">
         <v>48</v>
       </c>
-      <c r="J37" s="25" t="n">
-        <v>66</v>
+      <c r="J37" s="24" t="n">
+        <v>70</v>
       </c>
       <c r="K37" s="24" t="n">
         <v>76</v>
@@ -3776,7 +3776,7 @@
         <v>8</v>
       </c>
       <c r="J38" s="26" t="n">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="K38" s="26" t="n">
         <v>14</v>
@@ -3788,241 +3788,241 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Orlando-Kissimmee-Sanford</t>
+          <t>San Jose-Sunnyvale-Santa Clara</t>
         </is>
       </c>
       <c r="B39" s="23" t="n">
         <v>41</v>
       </c>
       <c r="C39" s="26" t="n">
-        <v>48</v>
-      </c>
-      <c r="D39" s="26" t="n">
-        <v>48</v>
-      </c>
-      <c r="E39" s="26" t="n">
-        <v>36</v>
-      </c>
-      <c r="F39" s="26" t="n">
-        <v>32</v>
-      </c>
-      <c r="G39" s="24" t="n">
-        <v>90</v>
-      </c>
-      <c r="H39" s="26" t="n">
-        <v>20</v>
-      </c>
-      <c r="I39" s="26" t="n">
-        <v>44</v>
-      </c>
-      <c r="J39" s="24" t="n">
-        <v>74</v>
+        <v>24</v>
+      </c>
+      <c r="D39" s="25" t="n">
+        <v>54</v>
+      </c>
+      <c r="E39" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="26" t="n">
+        <v>40</v>
+      </c>
+      <c r="H39" s="25" t="n">
+        <v>60</v>
+      </c>
+      <c r="I39" s="24" t="n">
+        <v>96</v>
+      </c>
+      <c r="J39" s="25" t="n">
+        <v>62</v>
       </c>
       <c r="K39" s="26" t="n">
-        <v>18</v>
-      </c>
-      <c r="L39" s="26" t="n">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="L39" s="24" t="n">
+        <v>84</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Orlando-Kissimmee-Sanford</t>
         </is>
       </c>
       <c r="B40" s="23" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40" s="26" t="n">
+        <v>48</v>
+      </c>
+      <c r="D40" s="26" t="n">
+        <v>48</v>
+      </c>
+      <c r="E40" s="26" t="n">
+        <v>36</v>
+      </c>
+      <c r="F40" s="26" t="n">
         <v>32</v>
       </c>
-      <c r="D40" s="26" t="n">
-        <v>14</v>
-      </c>
-      <c r="E40" s="24" t="n">
-        <v>98</v>
-      </c>
-      <c r="F40" s="24" t="n">
-        <v>76</v>
-      </c>
-      <c r="G40" s="26" t="n">
-        <v>22</v>
+      <c r="G40" s="24" t="n">
+        <v>90</v>
       </c>
       <c r="H40" s="26" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I40" s="26" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J40" s="25" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K40" s="26" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L40" s="26" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Charlotte-Concord-Gastonia</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="B41" s="23" t="n">
-        <v>39</v>
-      </c>
-      <c r="C41" s="25" t="n">
-        <v>62</v>
-      </c>
-      <c r="D41" s="25" t="n">
-        <v>50</v>
-      </c>
-      <c r="E41" s="26" t="n">
-        <v>16</v>
-      </c>
-      <c r="F41" s="26" t="n">
-        <v>26</v>
-      </c>
-      <c r="G41" s="24" t="n">
-        <v>92</v>
+        <v>40</v>
+      </c>
+      <c r="C41" s="26" t="n">
+        <v>32</v>
+      </c>
+      <c r="D41" s="26" t="n">
+        <v>14</v>
+      </c>
+      <c r="E41" s="24" t="n">
+        <v>98</v>
+      </c>
+      <c r="F41" s="24" t="n">
+        <v>76</v>
+      </c>
+      <c r="G41" s="26" t="n">
+        <v>22</v>
       </c>
       <c r="H41" s="26" t="n">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="I41" s="26" t="n">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="J41" s="26" t="n">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="K41" s="26" t="n">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="L41" s="26" t="n">
-        <v>30</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>San Jose-Sunnyvale-Santa Clara</t>
+          <t>Charlotte-Concord-Gastonia</t>
         </is>
       </c>
       <c r="B42" s="23" t="n">
         <v>39</v>
       </c>
-      <c r="C42" s="26" t="n">
-        <v>24</v>
+      <c r="C42" s="25" t="n">
+        <v>62</v>
       </c>
       <c r="D42" s="25" t="n">
-        <v>54</v>
-      </c>
-      <c r="E42" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="G42" s="26" t="n">
-        <v>40</v>
-      </c>
-      <c r="H42" s="25" t="n">
-        <v>60</v>
-      </c>
-      <c r="I42" s="24" t="n">
-        <v>96</v>
+        <v>50</v>
+      </c>
+      <c r="E42" s="26" t="n">
+        <v>16</v>
+      </c>
+      <c r="F42" s="26" t="n">
+        <v>26</v>
+      </c>
+      <c r="G42" s="24" t="n">
+        <v>92</v>
+      </c>
+      <c r="H42" s="26" t="n">
+        <v>6</v>
+      </c>
+      <c r="I42" s="26" t="n">
+        <v>36</v>
       </c>
       <c r="J42" s="26" t="n">
+        <v>28</v>
+      </c>
+      <c r="K42" s="26" t="n">
         <v>48</v>
       </c>
-      <c r="K42" s="26" t="n">
-        <v>10</v>
-      </c>
-      <c r="L42" s="24" t="n">
-        <v>84</v>
+      <c r="L42" s="26" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Las Vegas-Henderson-North Las Vegas</t>
+          <t>Fresno</t>
         </is>
       </c>
       <c r="B43" s="23" t="n">
         <v>35</v>
       </c>
-      <c r="C43" s="26" t="n">
-        <v>6</v>
+      <c r="C43" s="27" t="n">
+        <v>0</v>
       </c>
       <c r="D43" s="26" t="n">
-        <v>36</v>
-      </c>
-      <c r="E43" s="24" t="n">
-        <v>80</v>
+        <v>18</v>
+      </c>
+      <c r="E43" s="25" t="n">
+        <v>58</v>
       </c>
       <c r="F43" s="26" t="n">
+        <v>22</v>
+      </c>
+      <c r="G43" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="26" t="n">
         <v>34</v>
       </c>
-      <c r="G43" s="24" t="n">
-        <v>74</v>
-      </c>
-      <c r="H43" s="25" t="n">
-        <v>52</v>
-      </c>
-      <c r="I43" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="J43" s="26" t="n">
-        <v>22</v>
+      <c r="I43" s="24" t="n">
+        <v>92</v>
+      </c>
+      <c r="J43" s="25" t="n">
+        <v>60</v>
       </c>
       <c r="K43" s="26" t="n">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="L43" s="26" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Fresno</t>
+          <t>Las Vegas-Henderson-North Las Vegas</t>
         </is>
       </c>
       <c r="B44" s="23" t="n">
-        <v>35</v>
-      </c>
-      <c r="C44" s="27" t="n">
+        <v>34</v>
+      </c>
+      <c r="C44" s="26" t="n">
+        <v>6</v>
+      </c>
+      <c r="D44" s="26" t="n">
+        <v>36</v>
+      </c>
+      <c r="E44" s="24" t="n">
+        <v>80</v>
+      </c>
+      <c r="F44" s="26" t="n">
+        <v>34</v>
+      </c>
+      <c r="G44" s="24" t="n">
+        <v>74</v>
+      </c>
+      <c r="H44" s="25" t="n">
+        <v>52</v>
+      </c>
+      <c r="I44" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="D44" s="26" t="n">
-        <v>18</v>
-      </c>
-      <c r="E44" s="25" t="n">
-        <v>58</v>
-      </c>
-      <c r="F44" s="26" t="n">
-        <v>22</v>
-      </c>
-      <c r="G44" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H44" s="26" t="n">
-        <v>34</v>
-      </c>
-      <c r="I44" s="24" t="n">
-        <v>92</v>
-      </c>
-      <c r="J44" s="25" t="n">
-        <v>54</v>
+      <c r="J44" s="26" t="n">
+        <v>14</v>
       </c>
       <c r="K44" s="26" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="L44" s="26" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45">
@@ -4096,7 +4096,7 @@
         <v>28</v>
       </c>
       <c r="J46" s="26" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K46" s="26" t="n">
         <v>22</v>
@@ -4108,81 +4108,81 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>New York Newark-Jersey City</t>
+          <t>Los Angeles-Long Beach-Anaheim</t>
         </is>
       </c>
       <c r="B47" s="23" t="n">
         <v>28</v>
       </c>
       <c r="C47" s="26" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D47" s="26" t="n">
-        <v>32</v>
-      </c>
-      <c r="E47" s="24" t="n">
-        <v>70</v>
+        <v>34</v>
+      </c>
+      <c r="E47" s="25" t="n">
+        <v>52</v>
       </c>
       <c r="F47" s="26" t="n">
-        <v>12</v>
-      </c>
-      <c r="G47" s="25" t="n">
-        <v>56</v>
-      </c>
-      <c r="H47" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="I47" s="26" t="n">
+        <v>4</v>
+      </c>
+      <c r="G47" s="26" t="n">
+        <v>16</v>
+      </c>
+      <c r="H47" s="26" t="n">
+        <v>30</v>
+      </c>
+      <c r="I47" s="25" t="n">
+        <v>64</v>
+      </c>
+      <c r="J47" s="26" t="n">
+        <v>24</v>
+      </c>
+      <c r="K47" s="26" t="n">
         <v>22</v>
       </c>
-      <c r="J47" s="26" t="n">
-        <v>46</v>
-      </c>
-      <c r="K47" s="26" t="n">
-        <v>6</v>
-      </c>
-      <c r="L47" s="25" t="n">
-        <v>50</v>
+      <c r="L47" s="26" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Los Angeles-Long Beach-Anaheim</t>
+          <t>New York Newark-Jersey City</t>
         </is>
       </c>
       <c r="B48" s="23" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C48" s="26" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D48" s="26" t="n">
-        <v>34</v>
-      </c>
-      <c r="E48" s="25" t="n">
-        <v>52</v>
+        <v>32</v>
+      </c>
+      <c r="E48" s="24" t="n">
+        <v>70</v>
       </c>
       <c r="F48" s="26" t="n">
-        <v>4</v>
-      </c>
-      <c r="G48" s="26" t="n">
-        <v>16</v>
-      </c>
-      <c r="H48" s="26" t="n">
-        <v>30</v>
-      </c>
-      <c r="I48" s="25" t="n">
-        <v>64</v>
+        <v>12</v>
+      </c>
+      <c r="G48" s="25" t="n">
+        <v>56</v>
+      </c>
+      <c r="H48" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" s="26" t="n">
+        <v>22</v>
       </c>
       <c r="J48" s="26" t="n">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="K48" s="26" t="n">
-        <v>22</v>
-      </c>
-      <c r="L48" s="26" t="n">
-        <v>40</v>
+        <v>6</v>
+      </c>
+      <c r="L48" s="25" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="49">
@@ -4216,7 +4216,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="26" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K49" s="26" t="n">
         <v>4</v>
@@ -4256,7 +4256,7 @@
         <v>90</v>
       </c>
       <c r="J50" s="26" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K50" s="26" t="n">
         <v>16</v>
@@ -4296,7 +4296,7 @@
         <v>14</v>
       </c>
       <c r="J51" s="26" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="K51" s="26" t="n">
         <v>22</v>
@@ -4433,7 +4433,7 @@
         <v>10.49</v>
       </c>
       <c r="J2" s="27" t="n">
-        <v>15.01</v>
+        <v>10.86</v>
       </c>
       <c r="K2" s="27" t="n">
         <v>0.2</v>
@@ -4475,7 +4475,7 @@
         <v>5.24</v>
       </c>
       <c r="J3" s="27" t="n">
-        <v>16.15</v>
+        <v>14.37</v>
       </c>
       <c r="K3" s="27" t="n">
         <v>0</v>
@@ -4517,7 +4517,7 @@
         <v>22.78</v>
       </c>
       <c r="J4" s="27" t="n">
-        <v>10.55</v>
+        <v>7.88</v>
       </c>
       <c r="K4" s="27" t="n">
         <v>-0.38</v>
@@ -4529,91 +4529,91 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Hartford-West Hartford-East Hartford</t>
+          <t>Salt Lake City-Murray</t>
         </is>
       </c>
       <c r="B5" s="28" t="inlineStr">
         <is>
-          <t>65 (B+)</t>
+          <t>66 (B+)</t>
         </is>
       </c>
       <c r="C5" s="27" t="n">
-        <v>2.7</v>
+        <v>3.8</v>
       </c>
       <c r="D5" s="27" t="n">
-        <v>64.7</v>
+        <v>72.53</v>
       </c>
       <c r="E5" s="27" t="n">
-        <v>-0.49</v>
+        <v>3.22</v>
       </c>
       <c r="F5" s="27" t="n">
-        <v>3.51</v>
+        <v>5.31</v>
       </c>
       <c r="G5" s="27" t="n">
-        <v>2.6</v>
+        <v>4.34</v>
       </c>
       <c r="H5" s="27" t="n">
-        <v>33.8</v>
+        <v>35.4</v>
       </c>
       <c r="I5" s="27" t="n">
-        <v>16.13</v>
+        <v>36.31</v>
       </c>
       <c r="J5" s="27" t="n">
-        <v>28.07</v>
+        <v>6.26</v>
       </c>
       <c r="K5" s="27" t="n">
-        <v>-0.41</v>
+        <v>-0.76</v>
       </c>
       <c r="L5" s="27" t="n">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Milwaukee-Waukesha</t>
+          <t>Hartford-West Hartford-East Hartford</t>
         </is>
       </c>
       <c r="B6" s="28" t="inlineStr">
         <is>
-          <t>64 (B+)</t>
+          <t>65 (B+)</t>
         </is>
       </c>
       <c r="C6" s="27" t="n">
-        <v>3.7</v>
+        <v>2.7</v>
       </c>
       <c r="D6" s="27" t="n">
-        <v>64.09</v>
+        <v>64.7</v>
       </c>
       <c r="E6" s="27" t="n">
-        <v>2.34</v>
+        <v>-0.49</v>
       </c>
       <c r="F6" s="27" t="n">
-        <v>0.86</v>
+        <v>3.51</v>
       </c>
       <c r="G6" s="27" t="n">
-        <v>1.62</v>
+        <v>2.6</v>
       </c>
       <c r="H6" s="27" t="n">
-        <v>34.4</v>
+        <v>33.8</v>
       </c>
       <c r="I6" s="27" t="n">
-        <v>-16.64</v>
+        <v>16.13</v>
       </c>
       <c r="J6" s="27" t="n">
-        <v>22.05</v>
+        <v>26.71</v>
       </c>
       <c r="K6" s="27" t="n">
-        <v>5.71</v>
+        <v>-0.41</v>
       </c>
       <c r="L6" s="27" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Salt Lake City-Murray</t>
+          <t>Milwaukee-Waukesha</t>
         </is>
       </c>
       <c r="B7" s="28" t="inlineStr">
@@ -4622,40 +4622,40 @@
         </is>
       </c>
       <c r="C7" s="27" t="n">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="D7" s="27" t="n">
-        <v>72.53</v>
+        <v>64.09</v>
       </c>
       <c r="E7" s="27" t="n">
-        <v>3.22</v>
+        <v>2.34</v>
       </c>
       <c r="F7" s="27" t="n">
-        <v>5.31</v>
+        <v>0.86</v>
       </c>
       <c r="G7" s="27" t="n">
-        <v>4.34</v>
+        <v>1.62</v>
       </c>
       <c r="H7" s="27" t="n">
-        <v>35.4</v>
+        <v>34.4</v>
       </c>
       <c r="I7" s="27" t="n">
-        <v>36.31</v>
+        <v>-16.64</v>
       </c>
       <c r="J7" s="27" t="n">
-        <v>4.42</v>
+        <v>21.59</v>
       </c>
       <c r="K7" s="27" t="n">
-        <v>-0.76</v>
+        <v>5.71</v>
       </c>
       <c r="L7" s="27" t="n">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Grand Rapids-Wyoming-Kentwood</t>
+          <t>Louisville-Jefferson County</t>
         </is>
       </c>
       <c r="B8" s="28" t="inlineStr">
@@ -4664,76 +4664,76 @@
         </is>
       </c>
       <c r="C8" s="27" t="n">
-        <v>4.8</v>
+        <v>4</v>
       </c>
       <c r="D8" s="27" t="n">
-        <v>65.59999999999999</v>
+        <v>63.02</v>
       </c>
       <c r="E8" s="27" t="n">
-        <v>4.35</v>
+        <v>2.51</v>
       </c>
       <c r="F8" s="27" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.91</v>
       </c>
       <c r="G8" s="27" t="n">
-        <v>1.74</v>
+        <v>2.06</v>
       </c>
       <c r="H8" s="27" t="n">
-        <v>34.8</v>
+        <v>34.2</v>
       </c>
       <c r="I8" s="27" t="n">
-        <v>-8.640000000000001</v>
+        <v>18.48</v>
       </c>
       <c r="J8" s="27" t="n">
-        <v>20.55</v>
+        <v>16.45</v>
       </c>
       <c r="K8" s="27" t="n">
-        <v>5</v>
+        <v>2.3</v>
       </c>
       <c r="L8" s="27" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Louisville-Jefferson County</t>
+          <t>Grand Rapids-Wyoming-Kentwood</t>
         </is>
       </c>
       <c r="B9" s="28" t="inlineStr">
         <is>
-          <t>61 (B+)</t>
+          <t>62 (B+)</t>
         </is>
       </c>
       <c r="C9" s="27" t="n">
-        <v>4</v>
+        <v>4.8</v>
       </c>
       <c r="D9" s="27" t="n">
-        <v>63.02</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="E9" s="27" t="n">
-        <v>2.51</v>
+        <v>4.35</v>
       </c>
       <c r="F9" s="27" t="n">
-        <v>0.91</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="G9" s="27" t="n">
-        <v>2.06</v>
+        <v>1.74</v>
       </c>
       <c r="H9" s="27" t="n">
-        <v>34.2</v>
+        <v>34.8</v>
       </c>
       <c r="I9" s="27" t="n">
-        <v>18.48</v>
+        <v>-8.640000000000001</v>
       </c>
       <c r="J9" s="27" t="n">
-        <v>16.45</v>
+        <v>19.4</v>
       </c>
       <c r="K9" s="27" t="n">
-        <v>2.3</v>
+        <v>5</v>
       </c>
       <c r="L9" s="27" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10">
@@ -4769,7 +4769,7 @@
         <v>14.29</v>
       </c>
       <c r="J10" s="27" t="n">
-        <v>-0.09</v>
+        <v>-0.54</v>
       </c>
       <c r="K10" s="27" t="n">
         <v>0.08</v>
@@ -4811,7 +4811,7 @@
         <v>-38.63</v>
       </c>
       <c r="J11" s="27" t="n">
-        <v>19.64</v>
+        <v>19.13</v>
       </c>
       <c r="K11" s="27" t="n">
         <v>0.75</v>
@@ -4853,7 +4853,7 @@
         <v>10.29</v>
       </c>
       <c r="J12" s="27" t="n">
-        <v>16.91</v>
+        <v>17</v>
       </c>
       <c r="K12" s="27" t="n">
         <v>1.05</v>
@@ -4895,7 +4895,7 @@
         <v>5.26</v>
       </c>
       <c r="J13" s="27" t="n">
-        <v>18.59</v>
+        <v>18.58</v>
       </c>
       <c r="K13" s="27" t="n">
         <v>3.01</v>
@@ -4937,7 +4937,7 @@
         <v>-28.25</v>
       </c>
       <c r="J14" s="27" t="n">
-        <v>10.75</v>
+        <v>8.65</v>
       </c>
       <c r="K14" s="27" t="n">
         <v>-0.9</v>
@@ -4979,7 +4979,7 @@
         <v>13.55</v>
       </c>
       <c r="J15" s="27" t="n">
-        <v>-0.72</v>
+        <v>-0.64</v>
       </c>
       <c r="K15" s="27" t="n">
         <v>-3.57</v>
@@ -5021,7 +5021,7 @@
         <v>144.37</v>
       </c>
       <c r="J16" s="27" t="n">
-        <v>22.12</v>
+        <v>21.89</v>
       </c>
       <c r="K16" s="27" t="n">
         <v>2.79</v>
@@ -5063,7 +5063,7 @@
         <v>-20.77</v>
       </c>
       <c r="J17" s="27" t="n">
-        <v>0.17</v>
+        <v>-0.16</v>
       </c>
       <c r="K17" s="27" t="n">
         <v>-1.18</v>
@@ -5105,7 +5105,7 @@
         <v>-5.7</v>
       </c>
       <c r="J18" s="27" t="n">
-        <v>2.55</v>
+        <v>2.37</v>
       </c>
       <c r="K18" s="27" t="n">
         <v>-0.47</v>
@@ -5145,7 +5145,7 @@
         <v>14.96</v>
       </c>
       <c r="J19" s="27" t="n">
-        <v>4.67</v>
+        <v>4</v>
       </c>
       <c r="K19" s="27" t="n">
         <v>12.86</v>
@@ -5187,7 +5187,7 @@
         <v>-15.43</v>
       </c>
       <c r="J20" s="27" t="n">
-        <v>17.21</v>
+        <v>18.79</v>
       </c>
       <c r="K20" s="27" t="n">
         <v>0.8100000000000001</v>
@@ -5229,7 +5229,7 @@
         <v>1.56</v>
       </c>
       <c r="J21" s="27" t="n">
-        <v>15.41</v>
+        <v>10.88</v>
       </c>
       <c r="K21" s="27" t="n">
         <v>0.63</v>
@@ -5271,7 +5271,7 @@
         <v>4.08</v>
       </c>
       <c r="J22" s="27" t="n">
-        <v>-1.19</v>
+        <v>-1.32</v>
       </c>
       <c r="K22" s="27" t="n">
         <v>-1.78</v>
@@ -5313,7 +5313,7 @@
         <v>5.64</v>
       </c>
       <c r="J23" s="27" t="n">
-        <v>20.88</v>
+        <v>20</v>
       </c>
       <c r="K23" s="27" t="n">
         <v>2.14</v>
@@ -5355,7 +5355,7 @@
         <v>1.32</v>
       </c>
       <c r="J24" s="27" t="n">
-        <v>18.24</v>
+        <v>16.76</v>
       </c>
       <c r="K24" s="27" t="n">
         <v>-0.65</v>
@@ -5372,7 +5372,7 @@
       </c>
       <c r="B25" s="28" t="inlineStr">
         <is>
-          <t>50 (B)</t>
+          <t>51 (B)</t>
         </is>
       </c>
       <c r="C25" s="27" t="n">
@@ -5397,7 +5397,7 @@
         <v>11.46</v>
       </c>
       <c r="J25" s="27" t="n">
-        <v>5.89</v>
+        <v>5.46</v>
       </c>
       <c r="K25" s="27" t="n">
         <v>-0.16</v>
@@ -5409,7 +5409,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Detroit-Warren-Dearborn</t>
+          <t>Boston-Cambridge-Newton</t>
         </is>
       </c>
       <c r="B26" s="28" t="inlineStr">
@@ -5418,118 +5418,118 @@
         </is>
       </c>
       <c r="C26" s="27" t="n">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
       <c r="D26" s="27" t="n">
-        <v>60.93</v>
+        <v>68.47</v>
       </c>
       <c r="E26" s="27" t="n">
-        <v>4.58</v>
+        <v>2.1</v>
       </c>
       <c r="F26" s="27" t="n">
-        <v>4.75</v>
+        <v>6.46</v>
       </c>
       <c r="G26" s="27" t="n">
-        <v>1.72</v>
+        <v>2.94</v>
       </c>
       <c r="H26" s="27" t="n">
-        <v>34.7</v>
+        <v>33.5</v>
       </c>
       <c r="I26" s="27" t="n">
-        <v>57.77</v>
+        <v>-25.94</v>
       </c>
       <c r="J26" s="27" t="n">
-        <v>3.53</v>
+        <v>4.14</v>
       </c>
       <c r="K26" s="27" t="n">
-        <v>-1.09</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="L26" s="27" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Austin-Round Rock-San Marcos</t>
+          <t>Detroit-Warren-Dearborn</t>
         </is>
       </c>
       <c r="B27" s="28" t="inlineStr">
         <is>
-          <t>50 (B)</t>
+          <t>50 (B-)</t>
         </is>
       </c>
       <c r="C27" s="27" t="n">
-        <v>3.9</v>
+        <v>4.3</v>
       </c>
       <c r="D27" s="27" t="n">
-        <v>73.45999999999999</v>
+        <v>60.93</v>
       </c>
       <c r="E27" s="27" t="n">
-        <v>5.02</v>
+        <v>4.58</v>
       </c>
       <c r="F27" s="27" t="n">
-        <v>4.64</v>
+        <v>4.75</v>
       </c>
       <c r="G27" s="27" t="n">
-        <v>2.68</v>
+        <v>1.72</v>
       </c>
       <c r="H27" s="27" t="n">
-        <v>35.3</v>
+        <v>34.7</v>
       </c>
       <c r="I27" s="27" t="n">
-        <v>-37.08</v>
+        <v>57.77</v>
       </c>
       <c r="J27" s="27" t="n">
-        <v>-10.76</v>
+        <v>3.7</v>
       </c>
       <c r="K27" s="27" t="n">
-        <v>-4.23</v>
+        <v>-1.09</v>
       </c>
       <c r="L27" s="27" t="n">
-        <v>80</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Boston-Cambridge-Newton</t>
+          <t>Austin-Round Rock-San Marcos</t>
         </is>
       </c>
       <c r="B28" s="28" t="inlineStr">
         <is>
-          <t>49 (B-)</t>
+          <t>50 (B)</t>
         </is>
       </c>
       <c r="C28" s="27" t="n">
         <v>3.9</v>
       </c>
       <c r="D28" s="27" t="n">
-        <v>68.47</v>
+        <v>73.45999999999999</v>
       </c>
       <c r="E28" s="27" t="n">
-        <v>2.1</v>
+        <v>5.02</v>
       </c>
       <c r="F28" s="27" t="n">
-        <v>6.46</v>
+        <v>4.64</v>
       </c>
       <c r="G28" s="27" t="n">
-        <v>2.94</v>
+        <v>2.68</v>
       </c>
       <c r="H28" s="27" t="n">
-        <v>33.5</v>
+        <v>35.3</v>
       </c>
       <c r="I28" s="27" t="n">
-        <v>-25.94</v>
+        <v>-37.08</v>
       </c>
       <c r="J28" s="27" t="n">
-        <v>4.07</v>
+        <v>-10.3</v>
       </c>
       <c r="K28" s="27" t="n">
-        <v>0.9399999999999999</v>
+        <v>-4.23</v>
       </c>
       <c r="L28" s="27" t="n">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29">
@@ -5565,7 +5565,7 @@
         <v>-32</v>
       </c>
       <c r="J29" s="27" t="n">
-        <v>13.42</v>
+        <v>14.35</v>
       </c>
       <c r="K29" s="27" t="n">
         <v>2.48</v>
@@ -5607,7 +5607,7 @@
         <v>-24.33</v>
       </c>
       <c r="J30" s="27" t="n">
-        <v>16.85</v>
+        <v>15.05</v>
       </c>
       <c r="K30" s="27" t="n">
         <v>4.71</v>
@@ -5649,7 +5649,7 @@
         <v>76.97</v>
       </c>
       <c r="J31" s="27" t="n">
-        <v>-1.69</v>
+        <v>-1.26</v>
       </c>
       <c r="K31" s="27" t="n">
         <v>-3.51</v>
@@ -5661,7 +5661,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Phoenix-Mesa-Chandler</t>
+          <t>Tampa-St. Petersburg-Clearwater</t>
         </is>
       </c>
       <c r="B32" s="28" t="inlineStr">
@@ -5670,82 +5670,82 @@
         </is>
       </c>
       <c r="C32" s="27" t="n">
-        <v>4.2</v>
+        <v>4.4</v>
       </c>
       <c r="D32" s="27" t="n">
-        <v>65.47</v>
+        <v>60.12</v>
       </c>
       <c r="E32" s="27" t="n">
-        <v>5.17</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="F32" s="27" t="n">
-        <v>5.08</v>
+        <v>4.68</v>
       </c>
       <c r="G32" s="27" t="n">
-        <v>2.58</v>
+        <v>3</v>
       </c>
       <c r="H32" s="27" t="n">
-        <v>34.7</v>
+        <v>34.8</v>
       </c>
       <c r="I32" s="27" t="n">
-        <v>-21.38</v>
+        <v>10.06</v>
       </c>
       <c r="J32" s="27" t="n">
-        <v>-1.68</v>
+        <v>-4.14</v>
       </c>
       <c r="K32" s="27" t="n">
-        <v>-1.94</v>
+        <v>-0.4</v>
       </c>
       <c r="L32" s="27" t="n">
-        <v>58</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Tampa-St. Petersburg-Clearwater</t>
+          <t>Washington-Arlington-Alexandria</t>
         </is>
       </c>
       <c r="B33" s="28" t="inlineStr">
         <is>
-          <t>47 (B-)</t>
+          <t>46 (B-)</t>
         </is>
       </c>
       <c r="C33" s="27" t="n">
-        <v>4.4</v>
+        <v>4.3</v>
       </c>
       <c r="D33" s="27" t="n">
-        <v>60.12</v>
+        <v>68.17</v>
       </c>
       <c r="E33" s="27" t="n">
-        <v>8.640000000000001</v>
+        <v>1.83</v>
       </c>
       <c r="F33" s="27" t="n">
-        <v>4.68</v>
+        <v>5.2</v>
       </c>
       <c r="G33" s="27" t="n">
-        <v>3</v>
+        <v>2.28</v>
       </c>
       <c r="H33" s="27" t="n">
-        <v>34.8</v>
+        <v>34.7</v>
       </c>
       <c r="I33" s="27" t="n">
-        <v>10.06</v>
+        <v>2.42</v>
       </c>
       <c r="J33" s="27" t="n">
-        <v>-3.34</v>
+        <v>0.67</v>
       </c>
       <c r="K33" s="27" t="n">
-        <v>-0.4</v>
+        <v>-4.37</v>
       </c>
       <c r="L33" s="27" t="n">
-        <v>79</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Washington-Arlington-Alexandria</t>
+          <t>Phoenix-Mesa-Chandler</t>
         </is>
       </c>
       <c r="B34" s="28" t="inlineStr">
@@ -5754,34 +5754,34 @@
         </is>
       </c>
       <c r="C34" s="27" t="n">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="D34" s="27" t="n">
-        <v>68.17</v>
+        <v>65.47</v>
       </c>
       <c r="E34" s="27" t="n">
-        <v>1.83</v>
+        <v>5.17</v>
       </c>
       <c r="F34" s="27" t="n">
-        <v>5.2</v>
+        <v>5.08</v>
       </c>
       <c r="G34" s="27" t="n">
-        <v>2.28</v>
+        <v>2.58</v>
       </c>
       <c r="H34" s="27" t="n">
         <v>34.7</v>
       </c>
       <c r="I34" s="27" t="n">
-        <v>2.42</v>
+        <v>-21.38</v>
       </c>
       <c r="J34" s="27" t="n">
-        <v>0.91</v>
+        <v>-2.02</v>
       </c>
       <c r="K34" s="27" t="n">
-        <v>-4.37</v>
+        <v>-1.94</v>
       </c>
       <c r="L34" s="27" t="n">
-        <v>38</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35">
@@ -5792,7 +5792,7 @@
       </c>
       <c r="B35" s="28" t="inlineStr">
         <is>
-          <t>45 (B-)</t>
+          <t>44 (B-)</t>
         </is>
       </c>
       <c r="C35" s="27" t="n">
@@ -5817,7 +5817,7 @@
         <v>-6.1</v>
       </c>
       <c r="J35" s="27" t="n">
-        <v>10.73</v>
+        <v>8.48</v>
       </c>
       <c r="K35" s="27" t="n">
         <v>-1.71</v>
@@ -5834,7 +5834,7 @@
       </c>
       <c r="B36" s="28" t="inlineStr">
         <is>
-          <t>45 (B-)</t>
+          <t>44 (B-)</t>
         </is>
       </c>
       <c r="C36" s="27" t="n">
@@ -5859,7 +5859,7 @@
         <v>-34.38</v>
       </c>
       <c r="J36" s="27" t="n">
-        <v>9.220000000000001</v>
+        <v>5.21</v>
       </c>
       <c r="K36" s="27" t="n">
         <v>-0.21</v>
@@ -5901,7 +5901,7 @@
         <v>-0.88</v>
       </c>
       <c r="J37" s="27" t="n">
-        <v>14.33</v>
+        <v>14.25</v>
       </c>
       <c r="K37" s="27" t="n">
         <v>0.88</v>
@@ -5943,7 +5943,7 @@
         <v>-36.19</v>
       </c>
       <c r="J38" s="27" t="n">
-        <v>5.46</v>
+        <v>3.43</v>
       </c>
       <c r="K38" s="27" t="n">
         <v>-3.3</v>
@@ -5955,7 +5955,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Orlando-Kissimmee-Sanford</t>
+          <t>San Jose-Sunnyvale-Santa Clara</t>
         </is>
       </c>
       <c r="B39" s="28" t="inlineStr">
@@ -5964,124 +5964,124 @@
         </is>
       </c>
       <c r="C39" s="27" t="n">
-        <v>4.3</v>
+        <v>4.7</v>
       </c>
       <c r="D39" s="27" t="n">
-        <v>64.44</v>
+        <v>64.77</v>
       </c>
       <c r="E39" s="27" t="n">
-        <v>2.81</v>
+        <v>-0.88</v>
       </c>
       <c r="F39" s="27" t="n">
-        <v>5.26</v>
+        <v>7.66</v>
       </c>
       <c r="G39" s="27" t="n">
-        <v>3.9</v>
+        <v>2.14</v>
       </c>
       <c r="H39" s="27" t="n">
-        <v>33.5</v>
+        <v>34.4</v>
       </c>
       <c r="I39" s="27" t="n">
-        <v>-3.79</v>
+        <v>90.23</v>
       </c>
       <c r="J39" s="27" t="n">
-        <v>16.16</v>
+        <v>9.58</v>
       </c>
       <c r="K39" s="27" t="n">
-        <v>-2.83</v>
+        <v>-3.54</v>
       </c>
       <c r="L39" s="27" t="n">
-        <v>81</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Orlando-Kissimmee-Sanford</t>
         </is>
       </c>
       <c r="B40" s="28" t="inlineStr">
         <is>
-          <t>41 (B-)</t>
+          <t>40 (B-)</t>
         </is>
       </c>
       <c r="C40" s="27" t="n">
-        <v>4.6</v>
+        <v>4.3</v>
       </c>
       <c r="D40" s="27" t="n">
-        <v>60.61</v>
+        <v>64.44</v>
       </c>
       <c r="E40" s="27" t="n">
-        <v>9.66</v>
+        <v>2.81</v>
       </c>
       <c r="F40" s="27" t="n">
-        <v>4.4</v>
+        <v>5.26</v>
       </c>
       <c r="G40" s="27" t="n">
-        <v>1.72</v>
+        <v>3.9</v>
       </c>
       <c r="H40" s="27" t="n">
-        <v>33.6</v>
+        <v>33.5</v>
       </c>
       <c r="I40" s="27" t="n">
-        <v>-2.63</v>
+        <v>-3.79</v>
       </c>
       <c r="J40" s="27" t="n">
-        <v>12.27</v>
+        <v>10.12</v>
       </c>
       <c r="K40" s="27" t="n">
-        <v>-2.55</v>
+        <v>-2.83</v>
       </c>
       <c r="L40" s="27" t="n">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Charlotte-Concord-Gastonia</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="B41" s="28" t="inlineStr">
         <is>
-          <t>39 (C+)</t>
+          <t>40 (B-)</t>
         </is>
       </c>
       <c r="C41" s="27" t="n">
-        <v>4.1</v>
+        <v>4.6</v>
       </c>
       <c r="D41" s="27" t="n">
-        <v>64.69</v>
+        <v>60.61</v>
       </c>
       <c r="E41" s="27" t="n">
-        <v>1.59</v>
+        <v>9.66</v>
       </c>
       <c r="F41" s="27" t="n">
-        <v>5.36</v>
+        <v>4.4</v>
       </c>
       <c r="G41" s="27" t="n">
-        <v>4.1</v>
+        <v>1.72</v>
       </c>
       <c r="H41" s="27" t="n">
-        <v>33.2</v>
+        <v>33.6</v>
       </c>
       <c r="I41" s="27" t="n">
-        <v>-15.37</v>
+        <v>-2.63</v>
       </c>
       <c r="J41" s="27" t="n">
-        <v>1.59</v>
+        <v>5.54</v>
       </c>
       <c r="K41" s="27" t="n">
-        <v>-0.75</v>
+        <v>-2.55</v>
       </c>
       <c r="L41" s="27" t="n">
-        <v>59</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>San Jose-Sunnyvale-Santa Clara</t>
+          <t>Charlotte-Concord-Gastonia</t>
         </is>
       </c>
       <c r="B42" s="28" t="inlineStr">
@@ -6090,40 +6090,40 @@
         </is>
       </c>
       <c r="C42" s="27" t="n">
-        <v>4.7</v>
+        <v>4.1</v>
       </c>
       <c r="D42" s="27" t="n">
-        <v>64.77</v>
+        <v>64.69</v>
       </c>
       <c r="E42" s="27" t="n">
-        <v>-0.88</v>
+        <v>1.59</v>
       </c>
       <c r="F42" s="27" t="n">
-        <v>7.66</v>
+        <v>5.36</v>
       </c>
       <c r="G42" s="27" t="n">
-        <v>2.14</v>
+        <v>4.1</v>
       </c>
       <c r="H42" s="27" t="n">
-        <v>34.4</v>
+        <v>33.2</v>
       </c>
       <c r="I42" s="27" t="n">
-        <v>90.23</v>
+        <v>-15.37</v>
       </c>
       <c r="J42" s="27" t="n">
-        <v>6.95</v>
+        <v>0.73</v>
       </c>
       <c r="K42" s="27" t="n">
-        <v>-3.54</v>
+        <v>-0.75</v>
       </c>
       <c r="L42" s="27" t="n">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Las Vegas-Henderson-North Las Vegas</t>
+          <t>Fresno</t>
         </is>
       </c>
       <c r="B43" s="28" t="inlineStr">
@@ -6132,76 +6132,76 @@
         </is>
       </c>
       <c r="C43" s="27" t="n">
-        <v>5.6</v>
+        <v>7.9</v>
       </c>
       <c r="D43" s="27" t="n">
-        <v>63.62</v>
+        <v>60.66</v>
       </c>
       <c r="E43" s="27" t="n">
-        <v>6.47</v>
+        <v>4.59</v>
       </c>
       <c r="F43" s="27" t="n">
-        <v>5.22</v>
+        <v>5.44</v>
       </c>
       <c r="G43" s="27" t="n">
-        <v>3.04</v>
+        <v>0.12</v>
       </c>
       <c r="H43" s="27" t="n">
-        <v>34.2</v>
+        <v>33.8</v>
       </c>
       <c r="I43" s="27" t="n">
-        <v>-46.49</v>
+        <v>61.97</v>
       </c>
       <c r="J43" s="27" t="n">
-        <v>0.24</v>
+        <v>9.4</v>
       </c>
       <c r="K43" s="27" t="n">
-        <v>-1.12</v>
+        <v>-0.76</v>
       </c>
       <c r="L43" s="27" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Fresno</t>
+          <t>Las Vegas-Henderson-North Las Vegas</t>
         </is>
       </c>
       <c r="B44" s="28" t="inlineStr">
         <is>
-          <t>35 (C+)</t>
+          <t>34 (C+)</t>
         </is>
       </c>
       <c r="C44" s="27" t="n">
-        <v>7.9</v>
+        <v>5.6</v>
       </c>
       <c r="D44" s="27" t="n">
-        <v>60.66</v>
+        <v>63.62</v>
       </c>
       <c r="E44" s="27" t="n">
-        <v>4.59</v>
+        <v>6.47</v>
       </c>
       <c r="F44" s="27" t="n">
-        <v>5.44</v>
+        <v>5.22</v>
       </c>
       <c r="G44" s="27" t="n">
-        <v>0.12</v>
+        <v>3.04</v>
       </c>
       <c r="H44" s="27" t="n">
-        <v>33.8</v>
+        <v>34.2</v>
       </c>
       <c r="I44" s="27" t="n">
-        <v>61.97</v>
+        <v>-46.49</v>
       </c>
       <c r="J44" s="27" t="n">
-        <v>9.84</v>
+        <v>-0.71</v>
       </c>
       <c r="K44" s="27" t="n">
-        <v>-0.76</v>
+        <v>-1.12</v>
       </c>
       <c r="L44" s="27" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45">
@@ -6237,7 +6237,7 @@
         <v>-18.53</v>
       </c>
       <c r="J45" s="27" t="n">
-        <v>9.42</v>
+        <v>7.22</v>
       </c>
       <c r="K45" s="27" t="n">
         <v>-1.27</v>
@@ -6279,7 +6279,7 @@
         <v>-20.27</v>
       </c>
       <c r="J46" s="27" t="n">
-        <v>0.24</v>
+        <v>-0.24</v>
       </c>
       <c r="K46" s="27" t="n">
         <v>-2.11</v>
@@ -6291,7 +6291,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>New York Newark-Jersey City</t>
+          <t>Los Angeles-Long Beach-Anaheim</t>
         </is>
       </c>
       <c r="B47" s="28" t="inlineStr">
@@ -6300,76 +6300,76 @@
         </is>
       </c>
       <c r="C47" s="27" t="n">
-        <v>5.2</v>
+        <v>5.9</v>
       </c>
       <c r="D47" s="27" t="n">
-        <v>63.15</v>
+        <v>63.49</v>
       </c>
       <c r="E47" s="27" t="n">
-        <v>5.45</v>
+        <v>4.16</v>
       </c>
       <c r="F47" s="27" t="n">
-        <v>6.26</v>
+        <v>7.43</v>
       </c>
       <c r="G47" s="27" t="n">
-        <v>2.68</v>
+        <v>1.32</v>
       </c>
       <c r="H47" s="27" t="n">
-        <v>32.7</v>
+        <v>33.7</v>
       </c>
       <c r="I47" s="27" t="n">
-        <v>-21.86</v>
+        <v>6.1</v>
       </c>
       <c r="J47" s="27" t="n">
-        <v>6.08</v>
+        <v>0.36</v>
       </c>
       <c r="K47" s="27" t="n">
-        <v>-3.86</v>
+        <v>-2.11</v>
       </c>
       <c r="L47" s="27" t="n">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Los Angeles-Long Beach-Anaheim</t>
+          <t>New York Newark-Jersey City</t>
         </is>
       </c>
       <c r="B48" s="28" t="inlineStr">
         <is>
-          <t>28 (C)</t>
+          <t>27 (C)</t>
         </is>
       </c>
       <c r="C48" s="27" t="n">
-        <v>5.9</v>
+        <v>5.2</v>
       </c>
       <c r="D48" s="27" t="n">
-        <v>63.49</v>
+        <v>63.15</v>
       </c>
       <c r="E48" s="27" t="n">
-        <v>4.16</v>
+        <v>5.45</v>
       </c>
       <c r="F48" s="27" t="n">
-        <v>7.43</v>
+        <v>6.26</v>
       </c>
       <c r="G48" s="27" t="n">
-        <v>1.32</v>
+        <v>2.68</v>
       </c>
       <c r="H48" s="27" t="n">
-        <v>33.7</v>
+        <v>32.7</v>
       </c>
       <c r="I48" s="27" t="n">
-        <v>6.1</v>
+        <v>-21.86</v>
       </c>
       <c r="J48" s="27" t="n">
-        <v>-0.02</v>
+        <v>5.24</v>
       </c>
       <c r="K48" s="27" t="n">
-        <v>-2.11</v>
+        <v>-3.86</v>
       </c>
       <c r="L48" s="27" t="n">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49">
@@ -6405,7 +6405,7 @@
         <v>-39.96</v>
       </c>
       <c r="J49" s="27" t="n">
-        <v>-1.51</v>
+        <v>-0.83</v>
       </c>
       <c r="K49" s="27" t="n">
         <v>-4.22</v>
@@ -6447,7 +6447,7 @@
         <v>61.67</v>
       </c>
       <c r="J50" s="27" t="n">
-        <v>-0.67</v>
+        <v>-0.82</v>
       </c>
       <c r="K50" s="27" t="n">
         <v>-3.13</v>
@@ -6489,7 +6489,7 @@
         <v>-30.14</v>
       </c>
       <c r="J51" s="27" t="n">
-        <v>0.95</v>
+        <v>3.1</v>
       </c>
       <c r="K51" s="27" t="n">
         <v>-2.11</v>
@@ -6596,7 +6596,7 @@
         </is>
       </c>
       <c r="D2" s="17" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="18" t="inlineStr">
         <is>
@@ -6604,7 +6604,7 @@
         </is>
       </c>
       <c r="F2" s="17" t="n">
-        <v>27.5</v>
+        <v>27.3</v>
       </c>
       <c r="G2" s="17" t="n">
         <v>5.2</v>
@@ -6642,7 +6642,7 @@
         </is>
       </c>
       <c r="F3" s="17" t="n">
-        <v>27.5</v>
+        <v>28.1</v>
       </c>
       <c r="G3" s="17" t="n">
         <v>5.9</v>
@@ -6672,7 +6672,7 @@
         </is>
       </c>
       <c r="D4" s="8" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E4" s="9" t="inlineStr">
         <is>
@@ -6680,7 +6680,7 @@
         </is>
       </c>
       <c r="F4" s="8" t="n">
-        <v>50.4</v>
+        <v>50.6</v>
       </c>
       <c r="G4" s="8" t="n">
         <v>4.6</v>
@@ -6718,7 +6718,7 @@
         </is>
       </c>
       <c r="F5" s="8" t="n">
-        <v>52.2</v>
+        <v>51.8</v>
       </c>
       <c r="G5" s="8" t="n">
         <v>4.4</v>
@@ -6748,7 +6748,7 @@
         </is>
       </c>
       <c r="D6" s="11" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="12" t="inlineStr">
         <is>
@@ -6756,7 +6756,7 @@
         </is>
       </c>
       <c r="F6" s="11" t="n">
-        <v>44.6</v>
+        <v>44.4</v>
       </c>
       <c r="G6" s="11" t="n">
         <v>5</v>
@@ -6794,7 +6794,7 @@
         </is>
       </c>
       <c r="F7" s="11" t="n">
-        <v>48.1</v>
+        <v>48.5</v>
       </c>
       <c r="G7" s="11" t="n">
         <v>3.7</v>
@@ -6870,7 +6870,7 @@
         </is>
       </c>
       <c r="F9" s="8" t="n">
-        <v>54.1</v>
+        <v>54.3</v>
       </c>
       <c r="G9" s="8" t="n">
         <v>3.5</v>
@@ -6908,7 +6908,7 @@
         </is>
       </c>
       <c r="F10" s="11" t="n">
-        <v>42.1</v>
+        <v>42.5</v>
       </c>
       <c r="G10" s="11" t="n">
         <v>5.1</v>
@@ -6938,7 +6938,7 @@
         </is>
       </c>
       <c r="D11" s="11" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="12" t="inlineStr">
         <is>
@@ -6946,7 +6946,7 @@
         </is>
       </c>
       <c r="F11" s="11" t="n">
-        <v>46.6</v>
+        <v>46.4</v>
       </c>
       <c r="G11" s="11" t="n">
         <v>4.2</v>
@@ -6976,7 +6976,7 @@
         </is>
       </c>
       <c r="D12" s="11" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E12" s="12" t="inlineStr">
         <is>
@@ -6984,7 +6984,7 @@
         </is>
       </c>
       <c r="F12" s="11" t="n">
-        <v>49.4</v>
+        <v>49.8</v>
       </c>
       <c r="G12" s="11" t="n">
         <v>3.9</v>
@@ -7060,7 +7060,7 @@
         </is>
       </c>
       <c r="F14" s="17" t="n">
-        <v>24</v>
+        <v>24.2</v>
       </c>
       <c r="G14" s="17" t="n">
         <v>4.8</v>
@@ -7098,7 +7098,7 @@
         </is>
       </c>
       <c r="F15" s="11" t="n">
-        <v>49.7</v>
+        <v>49.9</v>
       </c>
       <c r="G15" s="11" t="n">
         <v>4.3</v>
@@ -7136,7 +7136,7 @@
         </is>
       </c>
       <c r="F16" s="8" t="n">
-        <v>59.1</v>
+        <v>59.3</v>
       </c>
       <c r="G16" s="8" t="n">
         <v>4.6</v>
@@ -7174,7 +7174,7 @@
         </is>
       </c>
       <c r="F17" s="8" t="n">
-        <v>53.8</v>
+        <v>53.6</v>
       </c>
       <c r="G17" s="8" t="n">
         <v>4.1</v>
@@ -7250,7 +7250,7 @@
         </is>
       </c>
       <c r="F19" s="17" t="n">
-        <v>24.2</v>
+        <v>24</v>
       </c>
       <c r="G19" s="17" t="n">
         <v>5</v>
@@ -7288,7 +7288,7 @@
         </is>
       </c>
       <c r="F20" s="8" t="n">
-        <v>55</v>
+        <v>55.4</v>
       </c>
       <c r="G20" s="8" t="n">
         <v>3.7</v>
@@ -7318,7 +7318,7 @@
         </is>
       </c>
       <c r="D21" s="11" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E21" s="12" t="inlineStr">
         <is>
@@ -7326,7 +7326,7 @@
         </is>
       </c>
       <c r="F21" s="11" t="n">
-        <v>41.4</v>
+        <v>40.4</v>
       </c>
       <c r="G21" s="11" t="n">
         <v>4.3</v>
@@ -7364,7 +7364,7 @@
         </is>
       </c>
       <c r="F22" s="14" t="n">
-        <v>39.1</v>
+        <v>38.9</v>
       </c>
       <c r="G22" s="14" t="n">
         <v>4.1</v>
@@ -7402,7 +7402,7 @@
         </is>
       </c>
       <c r="F23" s="11" t="n">
-        <v>48.6</v>
+        <v>49.4</v>
       </c>
       <c r="G23" s="11" t="n">
         <v>4.3</v>
@@ -7440,7 +7440,7 @@
         </is>
       </c>
       <c r="F24" s="8" t="n">
-        <v>52.8</v>
+        <v>53.2</v>
       </c>
       <c r="G24" s="8" t="n">
         <v>4.5</v>
@@ -7478,7 +7478,7 @@
         </is>
       </c>
       <c r="F25" s="11" t="n">
-        <v>42.5</v>
+        <v>41.7</v>
       </c>
       <c r="G25" s="11" t="n">
         <v>4.4</v>
@@ -7554,7 +7554,7 @@
         </is>
       </c>
       <c r="F27" s="14" t="n">
-        <v>30.5</v>
+        <v>30.3</v>
       </c>
       <c r="G27" s="14" t="n">
         <v>5.3</v>
@@ -7592,7 +7592,7 @@
         </is>
       </c>
       <c r="F28" s="20" t="n">
-        <v>19.5</v>
+        <v>19.9</v>
       </c>
       <c r="G28" s="20" t="n">
         <v>5.4</v>
@@ -7630,7 +7630,7 @@
         </is>
       </c>
       <c r="F29" s="11" t="n">
-        <v>49.2</v>
+        <v>49</v>
       </c>
       <c r="G29" s="11" t="n">
         <v>4.7</v>
@@ -7660,7 +7660,7 @@
         </is>
       </c>
       <c r="D30" s="14" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E30" s="15" t="inlineStr">
         <is>
@@ -7668,7 +7668,7 @@
         </is>
       </c>
       <c r="F30" s="14" t="n">
-        <v>34.6</v>
+        <v>33.8</v>
       </c>
       <c r="G30" s="14" t="n">
         <v>5.6</v>
@@ -7744,7 +7744,7 @@
         </is>
       </c>
       <c r="F32" s="8" t="n">
-        <v>56</v>
+        <v>56.2</v>
       </c>
       <c r="G32" s="8" t="n">
         <v>4.3</v>
@@ -7782,7 +7782,7 @@
         </is>
       </c>
       <c r="F33" s="8" t="n">
-        <v>52.4</v>
+        <v>52</v>
       </c>
       <c r="G33" s="8" t="n">
         <v>4.7</v>
@@ -7820,7 +7820,7 @@
         </is>
       </c>
       <c r="F34" s="5" t="n">
-        <v>68.09999999999999</v>
+        <v>68.3</v>
       </c>
       <c r="G34" s="5" t="n">
         <v>3.6</v>
@@ -7858,7 +7858,7 @@
         </is>
       </c>
       <c r="F35" s="8" t="n">
-        <v>53.7</v>
+        <v>53.5</v>
       </c>
       <c r="G35" s="8" t="n">
         <v>3.4</v>
@@ -7894,7 +7894,7 @@
         </is>
       </c>
       <c r="F36" s="5" t="n">
-        <v>67</v>
+        <v>66.8</v>
       </c>
       <c r="G36" s="5" t="n">
         <v>3.1</v>
@@ -7910,40 +7910,40 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="14" t="n">
+      <c r="A37" s="11" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="15" t="inlineStr">
+      <c r="B37" s="12" t="inlineStr">
         <is>
           <t>San Jose-Sunnyvale-Santa Clara</t>
         </is>
       </c>
-      <c r="C37" s="15" t="inlineStr">
+      <c r="C37" s="12" t="inlineStr">
         <is>
           <t>San Jose</t>
         </is>
       </c>
-      <c r="D37" s="14" t="n">
-        <v>39</v>
-      </c>
-      <c r="E37" s="15" t="inlineStr">
-        <is>
-          <t>C+</t>
-        </is>
-      </c>
-      <c r="F37" s="14" t="n">
-        <v>39.3</v>
-      </c>
-      <c r="G37" s="14" t="n">
+      <c r="D37" s="11" t="n">
+        <v>41</v>
+      </c>
+      <c r="E37" s="12" t="inlineStr">
+        <is>
+          <t>B-</t>
+        </is>
+      </c>
+      <c r="F37" s="11" t="n">
+        <v>40.7</v>
+      </c>
+      <c r="G37" s="11" t="n">
         <v>4.7</v>
       </c>
-      <c r="H37" s="14" t="n">
+      <c r="H37" s="11" t="n">
         <v>64.77</v>
       </c>
-      <c r="I37" s="14" t="n">
+      <c r="I37" s="11" t="n">
         <v>-0.88</v>
       </c>
-      <c r="J37" s="14" t="n">
+      <c r="J37" s="11" t="n">
         <v>7.66</v>
       </c>
     </row>
@@ -7970,7 +7970,7 @@
         </is>
       </c>
       <c r="F38" s="8" t="n">
-        <v>55.7</v>
+        <v>55.5</v>
       </c>
       <c r="G38" s="8" t="n">
         <v>4</v>
@@ -8000,7 +8000,7 @@
         </is>
       </c>
       <c r="D39" s="11" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E39" s="12" t="inlineStr">
         <is>
@@ -8008,7 +8008,7 @@
         </is>
       </c>
       <c r="F39" s="11" t="n">
-        <v>41.4</v>
+        <v>40</v>
       </c>
       <c r="G39" s="11" t="n">
         <v>4.6</v>
@@ -8122,7 +8122,7 @@
         </is>
       </c>
       <c r="F42" s="8" t="n">
-        <v>56.2</v>
+        <v>56</v>
       </c>
       <c r="G42" s="8" t="n">
         <v>3.5</v>
@@ -8160,7 +8160,7 @@
         </is>
       </c>
       <c r="F43" s="2" t="n">
-        <v>72.90000000000001</v>
+        <v>72.7</v>
       </c>
       <c r="G43" s="2" t="n">
         <v>3.3</v>
@@ -8190,7 +8190,7 @@
         </is>
       </c>
       <c r="D44" s="5" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E44" s="6" t="inlineStr">
         <is>
@@ -8198,7 +8198,7 @@
         </is>
       </c>
       <c r="F44" s="5" t="n">
-        <v>61.4</v>
+        <v>61.6</v>
       </c>
       <c r="G44" s="5" t="n">
         <v>4</v>
@@ -8266,7 +8266,7 @@
         </is>
       </c>
       <c r="D46" s="11" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E46" s="12" t="inlineStr">
         <is>
@@ -8274,7 +8274,7 @@
         </is>
       </c>
       <c r="F46" s="11" t="n">
-        <v>44.7</v>
+        <v>43.9</v>
       </c>
       <c r="G46" s="11" t="n">
         <v>4.6</v>
@@ -8304,7 +8304,7 @@
         </is>
       </c>
       <c r="D47" s="5" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E47" s="6" t="inlineStr">
         <is>
@@ -8312,7 +8312,7 @@
         </is>
       </c>
       <c r="F47" s="5" t="n">
-        <v>64.3</v>
+        <v>65.5</v>
       </c>
       <c r="G47" s="5" t="n">
         <v>3.8</v>
@@ -8350,7 +8350,7 @@
         </is>
       </c>
       <c r="F48" s="8" t="n">
-        <v>52.9</v>
+        <v>52.7</v>
       </c>
       <c r="G48" s="8" t="n">
         <v>2.5</v>
@@ -8388,7 +8388,7 @@
         </is>
       </c>
       <c r="F49" s="14" t="n">
-        <v>34.6</v>
+        <v>35.2</v>
       </c>
       <c r="G49" s="14" t="n">
         <v>7.9</v>
@@ -8584,7 +8584,7 @@
       </c>
       <c r="F3" s="34" t="inlineStr">
         <is>
-          <t>San Jose-Sunnyvale-Santa Clara</t>
+          <t>Charlotte-Concord-Gastonia</t>
         </is>
       </c>
       <c r="G3" s="34" t="n">
@@ -8618,7 +8618,7 @@
       </c>
       <c r="F4" s="34" t="inlineStr">
         <is>
-          <t>Las Vegas-Henderson-North Las Vegas</t>
+          <t>Fresno</t>
         </is>
       </c>
       <c r="G4" s="34" t="n">
@@ -8652,11 +8652,11 @@
       </c>
       <c r="F5" s="34" t="inlineStr">
         <is>
-          <t>Fresno</t>
+          <t>Las Vegas-Henderson-North Las Vegas</t>
         </is>
       </c>
       <c r="G5" s="34" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="34" t="inlineStr">
         <is>
@@ -8670,11 +8670,11 @@
       </c>
       <c r="B6" s="33" t="inlineStr">
         <is>
-          <t>Hartford-West Hartford-East Hartford</t>
+          <t>Salt Lake City-Murray</t>
         </is>
       </c>
       <c r="C6" s="33" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D6" s="33" t="inlineStr">
         <is>
@@ -8704,11 +8704,11 @@
       </c>
       <c r="B7" s="33" t="inlineStr">
         <is>
-          <t>Milwaukee-Waukesha</t>
+          <t>Hartford-West Hartford-East Hartford</t>
         </is>
       </c>
       <c r="C7" s="33" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D7" s="33" t="inlineStr">
         <is>
@@ -8738,7 +8738,7 @@
       </c>
       <c r="B8" s="33" t="inlineStr">
         <is>
-          <t>Salt Lake City-Murray</t>
+          <t>Milwaukee-Waukesha</t>
         </is>
       </c>
       <c r="C8" s="33" t="n">
@@ -8754,7 +8754,7 @@
       </c>
       <c r="F8" s="34" t="inlineStr">
         <is>
-          <t>New York Newark-Jersey City</t>
+          <t>Los Angeles-Long Beach-Anaheim</t>
         </is>
       </c>
       <c r="G8" s="34" t="n">
@@ -8772,7 +8772,7 @@
       </c>
       <c r="B9" s="33" t="inlineStr">
         <is>
-          <t>Grand Rapids-Wyoming-Kentwood</t>
+          <t>Louisville-Jefferson County</t>
         </is>
       </c>
       <c r="C9" s="33" t="n">
@@ -8788,11 +8788,11 @@
       </c>
       <c r="F9" s="34" t="inlineStr">
         <is>
-          <t>Los Angeles-Long Beach-Anaheim</t>
+          <t>New York Newark-Jersey City</t>
         </is>
       </c>
       <c r="G9" s="34" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="34" t="inlineStr">
         <is>
@@ -8806,11 +8806,11 @@
       </c>
       <c r="B10" s="33" t="inlineStr">
         <is>
-          <t>Louisville-Jefferson County</t>
+          <t>Grand Rapids-Wyoming-Kentwood</t>
         </is>
       </c>
       <c r="C10" s="33" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D10" s="33" t="inlineStr">
         <is>

</xml_diff>